<commit_message>
added config folder and update depallet manager to handle the maguchi layout
</commit_message>
<xml_diff>
--- a/testing/デパレ間口_リン.xlsx
+++ b/testing/デパレ間口_リン.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\90181586\Downloads\デパレ間口ソースコード\デパレ間口ソースコード\20251107\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66A2F7F-6752-4629-9689-00F46FAA0CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760F48F4-B93A-474E-A5A0-23423E6A0D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="デパレ間口進捗" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
   <si>
     <t>件名</t>
   </si>
@@ -227,13 +227,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>○完了</t>
-  </si>
-  <si>
-    <t>○完了</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>デパレ間口 設備信号　Bライン側 R1</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -366,12 +359,225 @@
     </r>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>テスト</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>values</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>signal_id</t>
+  </si>
+  <si>
+    <t>signal_id</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オ069</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>タ０３３</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ア６１９</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>kanban_no</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>flow_rack 4444</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>間口5</t>
+    <rPh sb="0" eb="2">
+      <t>マグチ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>間口4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>間口3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>間口2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>間口1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>走る後、　values　１</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T632</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T436</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T622</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オ0７１</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>flow_rack 5555</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">flow_rack </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>走る後、　values1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>走る後、　values１</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承認</t>
+    <rPh sb="0" eb="2">
+      <t>ショウニン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>承認</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Bライン</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>取出数量</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>かんばん番号</t>
+    <rPh sb="4" eb="6">
+      <t>バンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T703</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T621</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T631</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T435</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T704</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>サ６０７</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">flow_rack6666 </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>帰る</t>
+    <rPh sb="0" eb="1">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>走る後、values１</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>take_count_map = {
+    "T703": "-9", "T621": "-1", "T631": "-2", "3237": "-2",
+    "オ070": "-1", "タ032": "-1", "オ068": "-1", "ア618": "-2",
+    "T435": "-2", "T704": "ー９", "T622": "-1", "T632": "-2",
+    "3238": "-2", "オ071": "-1", "タ033": "-1", "オ069": "-1",
+    "T436": "-2", "ア619": "-2", "サ607": "-2"
+}</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オ070</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>タ032</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オ068</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ア618</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>オ071</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>タ033</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ア619</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>サ607</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,13 +640,6 @@
       <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="游ゴシック"/>
-      <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
@@ -466,8 +665,51 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,8 +734,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFBAFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -501,12 +785,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE2E6"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -521,18 +921,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -541,6 +937,69 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -879,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -909,27 +1368,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="10" customFormat="1" ht="409.6" ph="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s" ph="1">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="409.6" ph="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s" ph="1">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s" ph="1">
-        <v>37</v>
+      <c r="B2" s="9" t="s" ph="1">
+        <v>35</v>
       </c>
       <c r="C2" s="4" t="s" ph="1">
         <v>22</v>
       </c>
-      <c r="D2" s="10" t="s" ph="1">
+      <c r="D2" s="2" t="s" ph="1">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s" ph="1">
-        <v>34</v>
+      <c r="E2" s="8" t="s" ph="1">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="222" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" ph="1"/>
       <c r="B3" s="1" t="s" ph="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4" t="s" ph="1">
         <v>21</v>
@@ -952,20 +1411,20 @@
       <c r="D4" s="5" ph="1"/>
       <c r="E4" ph="1"/>
     </row>
-    <row r="5" spans="1:5" s="12" customFormat="1" ht="108" ph="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="13" t="s" ph="1">
+    <row r="5" spans="1:5" s="10" customFormat="1" ht="108" ph="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="11" t="s" ph="1">
+        <v>34</v>
+      </c>
+      <c r="C5" s="12" t="s" ph="1">
+        <v>16</v>
+      </c>
+      <c r="D5" s="10" t="s" ph="1">
         <v>36</v>
       </c>
-      <c r="C5" s="14" t="s" ph="1">
-        <v>16</v>
-      </c>
-      <c r="D5" s="12" t="s" ph="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="12" customFormat="1" ht="27" ph="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="13" ph="1"/>
-      <c r="C6" s="14" ph="1"/>
+    </row>
+    <row r="6" spans="1:5" s="10" customFormat="1" ht="27" ph="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="11" ph="1"/>
+      <c r="C6" s="12" ph="1"/>
     </row>
     <row r="7" spans="1:5" ht="27" x14ac:dyDescent="0.45">
       <c r="A7" ph="1"/>
@@ -996,13 +1455,13 @@
     <row r="9" spans="1:5" ht="27" x14ac:dyDescent="0.45">
       <c r="A9" ph="1"/>
       <c r="B9" t="s" ph="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s" ph="1">
         <v>19</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" ph="1"/>
     </row>
@@ -1039,70 +1498,1144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972A1951-796F-43B0-BAF2-5D4B9B88D3C1}">
-  <dimension ref="A2:B8"/>
+  <dimension ref="A2:K92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="41.59765625" customWidth="1"/>
-    <col min="2" max="2" width="22.796875" customWidth="1"/>
+    <col min="1" max="1" width="36.296875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="14.296875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="13" style="15" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="15" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="14.09765625" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="15"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="1:6" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.45">
+      <c r="A4" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="14" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="25">
+        <v>3238</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="32">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C8" s="32">
+        <v>206</v>
+      </c>
+      <c r="D8" s="32">
+        <v>205</v>
+      </c>
+      <c r="E8" s="32">
+        <v>203</v>
+      </c>
+      <c r="F8" s="32">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="32">
+        <v>8504</v>
+      </c>
+      <c r="C9" s="32">
+        <v>8503</v>
+      </c>
+      <c r="D9" s="32">
+        <v>8502</v>
+      </c>
+      <c r="E9" s="32">
+        <v>8501</v>
+      </c>
+      <c r="F9" s="32">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="25">
+        <v>1</v>
+      </c>
+      <c r="C10" s="25">
+        <v>1</v>
+      </c>
+      <c r="D10" s="25">
+        <v>1</v>
+      </c>
+      <c r="E10" s="25">
+        <v>1</v>
+      </c>
+      <c r="F10" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="25">
+        <v>8260</v>
+      </c>
+      <c r="C11" s="25">
+        <v>8246</v>
+      </c>
+      <c r="D11" s="25">
+        <v>8231</v>
+      </c>
+      <c r="E11" s="25">
+        <v>8216</v>
+      </c>
+      <c r="F11" s="25">
+        <v>8201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="32">
+        <v>0</v>
+      </c>
+      <c r="C12" s="32">
+        <v>0</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0</v>
+      </c>
+      <c r="E12" s="32">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="32">
+        <v>8262</v>
+      </c>
+      <c r="C13" s="32">
+        <v>8247</v>
+      </c>
+      <c r="D13" s="32">
+        <v>8232</v>
+      </c>
+      <c r="E13" s="32">
+        <v>8217</v>
+      </c>
+      <c r="F13" s="32">
+        <v>8202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="32">
+        <v>29</v>
+      </c>
+      <c r="C19" s="32">
+        <v>204</v>
+      </c>
+      <c r="D19" s="32">
+        <v>201</v>
+      </c>
+      <c r="E19" s="32">
+        <v>207</v>
+      </c>
+      <c r="F19" s="32">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="32">
+        <v>8504</v>
+      </c>
+      <c r="C20" s="32">
+        <v>8503</v>
+      </c>
+      <c r="D20" s="32">
+        <v>8502</v>
+      </c>
+      <c r="E20" s="32">
+        <v>8501</v>
+      </c>
+      <c r="F20" s="32">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="25">
+        <v>1</v>
+      </c>
+      <c r="C21" s="25">
+        <v>1</v>
+      </c>
+      <c r="D21" s="25">
+        <v>1</v>
+      </c>
+      <c r="E21" s="25">
+        <v>1</v>
+      </c>
+      <c r="F21" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="25">
+        <v>8260</v>
+      </c>
+      <c r="C22" s="25">
+        <v>8246</v>
+      </c>
+      <c r="D22" s="25">
+        <v>8231</v>
+      </c>
+      <c r="E22" s="25">
+        <v>8216</v>
+      </c>
+      <c r="F22" s="25">
+        <v>8201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="32">
+        <v>0</v>
+      </c>
+      <c r="C23" s="32">
+        <v>0</v>
+      </c>
+      <c r="D23" s="32">
+        <v>0</v>
+      </c>
+      <c r="E23" s="32">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32">
+        <v>0</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+    </row>
+    <row r="25" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
+      <c r="J25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="20" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25">
+        <v>300</v>
+      </c>
+      <c r="E30" s="25">
+        <v>200</v>
+      </c>
+      <c r="F30" s="25">
+        <v>31</v>
+      </c>
+      <c r="H30" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25">
+        <v>8502</v>
+      </c>
+      <c r="E31" s="25">
+        <v>8501</v>
+      </c>
+      <c r="F31" s="25">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A32" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25">
+        <v>1</v>
+      </c>
+      <c r="E32" s="25">
+        <v>1</v>
+      </c>
+      <c r="F32" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25">
+        <v>8231</v>
+      </c>
+      <c r="E33" s="25">
+        <v>8216</v>
+      </c>
+      <c r="F33" s="25">
+        <v>8200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25">
+        <v>0</v>
+      </c>
+      <c r="E34" s="25">
+        <v>0</v>
+      </c>
+      <c r="F34" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+    </row>
+    <row r="36" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A36" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="17"/>
+    </row>
+    <row r="38" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F38" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="25">
+        <v>107</v>
+      </c>
+      <c r="C41" s="25">
+        <v>103</v>
+      </c>
+      <c r="D41" s="25">
+        <v>105</v>
+      </c>
+      <c r="E41" s="25">
+        <v>106</v>
+      </c>
+      <c r="F41" s="25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="25">
+        <v>8404</v>
+      </c>
+      <c r="C42" s="25">
+        <v>8403</v>
+      </c>
+      <c r="D42" s="25">
+        <v>8402</v>
+      </c>
+      <c r="E42" s="25">
+        <v>8401</v>
+      </c>
+      <c r="F42" s="25">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="25">
+        <v>1</v>
+      </c>
+      <c r="C43" s="25">
+        <v>1</v>
+      </c>
+      <c r="D43" s="25">
+        <v>1</v>
+      </c>
+      <c r="E43" s="25">
+        <v>1</v>
+      </c>
+      <c r="F43" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="25">
+        <v>8061</v>
+      </c>
+      <c r="C44" s="25">
+        <v>8046</v>
+      </c>
+      <c r="D44" s="25">
+        <v>8031</v>
+      </c>
+      <c r="E44" s="25">
+        <v>8016</v>
+      </c>
+      <c r="F44" s="25">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="25">
+        <v>0</v>
+      </c>
+      <c r="C45" s="25">
+        <v>0</v>
+      </c>
+      <c r="D45" s="25">
+        <v>0</v>
+      </c>
+      <c r="E45" s="25">
+        <v>0</v>
+      </c>
+      <c r="F45" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A46" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="17"/>
+    </row>
+    <row r="48" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="49" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
+      <c r="B49" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="25">
+        <v>102</v>
+      </c>
+      <c r="C51" s="25">
+        <v>108</v>
+      </c>
+      <c r="D51" s="25">
+        <v>101</v>
+      </c>
+      <c r="E51" s="25">
+        <v>104</v>
+      </c>
+      <c r="F51" s="25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="25">
+        <v>8404</v>
+      </c>
+      <c r="C52" s="25">
+        <v>8403</v>
+      </c>
+      <c r="D52" s="25">
+        <v>8402</v>
+      </c>
+      <c r="E52" s="25">
+        <v>8401</v>
+      </c>
+      <c r="F52" s="25">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="25">
+        <v>1</v>
+      </c>
+      <c r="C53" s="25">
+        <v>1</v>
+      </c>
+      <c r="D53" s="25">
+        <v>1</v>
+      </c>
+      <c r="E53" s="25">
+        <v>1</v>
+      </c>
+      <c r="F53" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="25">
+        <v>8061</v>
+      </c>
+      <c r="C54" s="25">
+        <v>8046</v>
+      </c>
+      <c r="D54" s="25">
+        <v>8032</v>
+      </c>
+      <c r="E54" s="25">
+        <v>8016</v>
+      </c>
+      <c r="F54" s="25">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="25">
+        <v>0</v>
+      </c>
+      <c r="C55" s="25">
+        <v>0</v>
+      </c>
+      <c r="D55" s="25">
+        <v>0</v>
+      </c>
+      <c r="E55" s="25">
+        <v>0</v>
+      </c>
+      <c r="F55" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A56" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="17"/>
+    </row>
+    <row r="58" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="59" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F59" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F60" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="25">
+        <v>23</v>
+      </c>
+      <c r="C61" s="25">
+        <v>100</v>
+      </c>
+      <c r="D61" s="25">
+        <v>301</v>
+      </c>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="25">
+        <v>8404</v>
+      </c>
+      <c r="C62" s="25">
+        <v>8403</v>
+      </c>
+      <c r="D62" s="25">
+        <v>8402</v>
+      </c>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="25">
+        <v>1</v>
+      </c>
+      <c r="C63" s="25">
+        <v>1</v>
+      </c>
+      <c r="D63" s="25">
+        <v>1</v>
+      </c>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B64" s="25">
+        <v>8060</v>
+      </c>
+      <c r="C64" s="25">
+        <v>8046</v>
+      </c>
+      <c r="D64" s="25">
+        <v>8032</v>
+      </c>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" s="25">
+        <v>0</v>
+      </c>
+      <c r="C65" s="25">
+        <v>0</v>
+      </c>
+      <c r="D65" s="25">
+        <v>0</v>
+      </c>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+    </row>
+    <row r="66" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A66" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="17"/>
+    </row>
+    <row r="69" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="70" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A70" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B71" s="15">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" s="15">
+        <f>B75</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="15">
+        <v>3237</v>
+      </c>
+      <c r="B74" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="15">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A81" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A82" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B82" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A83" s="15">
+        <v>3238</v>
+      </c>
+      <c r="B83" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A84" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A85" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A86" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A87" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B87" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A88" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A89" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="198" x14ac:dyDescent="0.45">
+      <c r="A92" s="33" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
confirmed flowrack side and fixed it later
</commit_message>
<xml_diff>
--- a/testing/デパレ間口_リン.xlsx
+++ b/testing/デパレ間口_リン.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\90181586\Downloads\デパレ間口ソースコード\デパレ間口ソースコード\20251107\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760F48F4-B93A-474E-A5A0-23423E6A0D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA938E42-C003-43BF-BEA3-EE35352BFA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="デパレ間口進捗" sheetId="1" r:id="rId1"/>
@@ -906,7 +906,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1000,6 +1000,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1338,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1500,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972A1951-796F-43B0-BAF2-5D4B9B88D3C1}">
   <dimension ref="A2:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1532,22 +1535,22 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="34" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed flowrack data entry for R1,R2,R3,L1,L2,L3 to the database by step-kanban-no
</commit_message>
<xml_diff>
--- a/testing/デパレ間口_リン.xlsx
+++ b/testing/デパレ間口_リン.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\90181586\Downloads\デパレ間口ソースコード\デパレ間口ソースコード\20251107\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8090EC66-830E-4A29-99FB-7FDF60818592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5758DECF-5D73-4A45-B120-C746999DD5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="134">
   <si>
     <t>件名</t>
   </si>
@@ -406,10 +406,6 @@
   </si>
   <si>
     <t>承認</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Bライン</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -722,10 +718,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>m_product</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">car_model_id </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -778,15 +770,27 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>add 26</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>in car_model_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>create car_model_id &gt; flow_rack 4444</t>
+    <t>kotatus_status</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">add </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>デパレ間口 設備信号</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">　Bライン側 </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LH 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>update step_kanban_no &gt; flow_rack 4444</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -802,42 +806,27 @@
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>K30147,K30148,K30149,K30150</t>
+      <t>K30147,K30148</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>t_shelf_status</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>作成</t>
-    <rPh sb="0" eb="2">
-      <t>サクセイ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">,K30149,K30150 </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>t_shelf_status =</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フローラックに step_kanban_no 更新</t>
+    <rPh sb="23" eb="25">
+      <t>コウシン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>フローラックにcar_model_id 作成</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>kotatus_status</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>up - car_model_id</t>
+    <t>更新</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -845,7 +834,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1020,6 +1009,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -1270,7 +1268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1442,28 +1440,46 @@
     <xf numFmtId="0" fontId="19" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1824,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="30" t="s" ph="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" s="30" t="s" ph="1">
         <v>8</v>
@@ -1965,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972A1951-796F-43B0-BAF2-5D4B9B88D3C1}">
   <dimension ref="A2:O180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -1991,7 +2007,10 @@
     <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="1:10" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
-        <v>59</v>
+        <v>125</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
@@ -2000,8 +2019,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="14" t="s">
-        <v>26</v>
+      <c r="A6" s="68" t="s">
+        <v>127</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>45</v>
@@ -2022,7 +2041,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="56" t="s">
         <v>44</v>
@@ -2042,7 +2061,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="54" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>
@@ -2052,95 +2071,104 @@
       <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="64" t="s">
-        <v>127</v>
+      <c r="A9" s="70" t="s">
+        <v>128</v>
       </c>
       <c r="B9" s="60"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
       <c r="G9" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="44"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="J9" s="44"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="72" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="D11" s="72" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="72"/>
+      <c r="G11" s="63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="72" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="59" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="59" t="s">
+      <c r="C12" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" s="59" t="s">
-        <v>117</v>
-      </c>
-      <c r="F11" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="G11" s="65" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="65" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="59" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.45"/>
+      <c r="E12" s="72">
+        <v>2004</v>
+      </c>
+      <c r="F12" s="72"/>
+    </row>
+    <row r="13" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="72"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+    </row>
     <row r="14" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
       <c r="G14" s="57"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="67" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="68" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
+      <c r="A15" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="66"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
       <c r="J15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="56">
+      <c r="B16" s="74">
         <v>26</v>
       </c>
       <c r="C16" s="50">
@@ -2156,7 +2184,7 @@
         <v>208</v>
       </c>
       <c r="G16" s="44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J16" s="44"/>
     </row>
@@ -2164,7 +2192,7 @@
       <c r="A17" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="56">
+      <c r="B17" s="74">
         <v>8504</v>
       </c>
       <c r="C17" s="50">
@@ -2180,13 +2208,13 @@
         <v>8500</v>
       </c>
       <c r="G17" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J17" s="44"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
@@ -2239,7 +2267,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
@@ -2288,13 +2316,13 @@
         <v>8201</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H23" s="47"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
@@ -2345,13 +2373,13 @@
         <v>8202</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H26" s="47"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="49"/>
       <c r="C27" s="49"/>
@@ -2380,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
@@ -2403,13 +2431,13 @@
         <v>8500</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H29" s="47"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -2459,7 +2487,7 @@
         <v>8202</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H32" s="47"/>
     </row>
@@ -2476,32 +2504,32 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="H34" s="46"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="67"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="H35" s="46"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="61"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="61"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="67"/>
+      <c r="N35" s="67"/>
+      <c r="O35" s="67"/>
     </row>
     <row r="36" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="J36" s="61"/>
-      <c r="K36" s="61"/>
-      <c r="L36" s="61"/>
-      <c r="M36" s="61"/>
-      <c r="N36" s="61"/>
-      <c r="O36" s="61"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="67"/>
+      <c r="N36" s="67"/>
+      <c r="O36" s="67"/>
     </row>
     <row r="37" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
@@ -2522,12 +2550,12 @@
       <c r="F37" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J37" s="61"/>
-      <c r="K37" s="61"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="61"/>
-      <c r="O37" s="61"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="67"/>
+      <c r="N37" s="67"/>
+      <c r="O37" s="67"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="53" t="s">
@@ -2537,7 +2565,7 @@
         <v>53</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" s="53" t="s">
         <v>52</v>
@@ -2550,16 +2578,16 @@
       </c>
       <c r="G38" s="44"/>
       <c r="H38" s="44"/>
-      <c r="J38" s="61"/>
-      <c r="K38" s="61"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="61"/>
-      <c r="O38" s="61"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="67"/>
+      <c r="N38" s="67"/>
+      <c r="O38" s="67"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B39" s="49"/>
       <c r="C39" s="49"/>
@@ -2611,15 +2639,15 @@
         <v>8500</v>
       </c>
       <c r="G41" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H41" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B42" s="49"/>
       <c r="C42" s="49"/>
@@ -2675,7 +2703,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A45" s="49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" s="49"/>
       <c r="C45" s="49"/>
@@ -2731,13 +2759,13 @@
         <v>8201</v>
       </c>
       <c r="G47" s="44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H47" s="47"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B48" s="49"/>
       <c r="C48" s="49"/>
@@ -2766,7 +2794,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H49" s="47"/>
     </row>
@@ -2794,7 +2822,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B51" s="49"/>
       <c r="C51" s="49"/>
@@ -2823,10 +2851,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H52" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.45">
@@ -2852,7 +2880,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" s="49"/>
       <c r="C54" s="49"/>
@@ -2881,7 +2909,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H55" s="47"/>
     </row>
@@ -2984,20 +3012,20 @@
       <c r="B63" s="53"/>
       <c r="C63" s="53"/>
       <c r="D63" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E63" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="53" t="s">
         <v>67</v>
-      </c>
-      <c r="E63" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="F63" s="53" t="s">
-        <v>68</v>
       </c>
       <c r="G63" s="44"/>
       <c r="H63" s="44"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="49"/>
       <c r="C64" s="49"/>
@@ -3041,15 +3069,15 @@
         <v>8500</v>
       </c>
       <c r="G66" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H66" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B67" s="49"/>
       <c r="C67" s="49"/>
@@ -3097,7 +3125,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -3119,7 +3147,7 @@
         <v>0</v>
       </c>
       <c r="G71" s="44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H71" s="47"/>
     </row>
@@ -3142,7 +3170,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B73" s="49"/>
       <c r="C73" s="49"/>
@@ -3167,7 +3195,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H74" s="47"/>
     </row>
@@ -3191,7 +3219,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B76" s="49"/>
       <c r="C76" s="49"/>
@@ -3216,10 +3244,10 @@
         <v>0</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H77" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.45">
@@ -3241,7 +3269,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B79" s="49"/>
       <c r="C79" s="49"/>
@@ -3266,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H80" s="47"/>
     </row>
@@ -3342,7 +3370,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87" s="49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B87" s="49"/>
       <c r="C87" s="49"/>
@@ -3394,15 +3422,15 @@
         <v>8400</v>
       </c>
       <c r="G89" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H89" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A90" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B90" s="49"/>
       <c r="C90" s="49"/>
@@ -3458,7 +3486,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A93" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B93" s="17"/>
       <c r="C93" s="17"/>
@@ -3486,7 +3514,7 @@
         <v>8000</v>
       </c>
       <c r="G94" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H94" s="47"/>
     </row>
@@ -3513,7 +3541,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A96" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -3542,7 +3570,7 @@
         <v>8002</v>
       </c>
       <c r="G97" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H97" s="47"/>
     </row>
@@ -3570,7 +3598,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A99" s="49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B99" s="49"/>
       <c r="C99" s="49"/>
@@ -3599,10 +3627,10 @@
         <v>8400</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H100" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.45">
@@ -3628,7 +3656,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A102" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B102" s="49"/>
       <c r="C102" s="49"/>
@@ -3657,7 +3685,7 @@
         <v>8002</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H103" s="47"/>
     </row>
@@ -3752,7 +3780,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A111" s="49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B111" s="49"/>
       <c r="C111" s="49"/>
@@ -3804,15 +3832,15 @@
         <v>8400</v>
       </c>
       <c r="G113" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H113" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A114" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B114" s="49"/>
       <c r="C114" s="49"/>
@@ -3868,7 +3896,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A117" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B117" s="17"/>
       <c r="C117" s="17"/>
@@ -3896,13 +3924,13 @@
         <v>8000</v>
       </c>
       <c r="G118" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H118" s="47"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A119" s="48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B119" s="48">
         <v>0</v>
@@ -3923,7 +3951,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A120" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -3952,13 +3980,13 @@
         <v>8002</v>
       </c>
       <c r="G121" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H121" s="47"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A122" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B122" s="48">
         <v>1</v>
@@ -3980,7 +4008,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A123" s="49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B123" s="49"/>
       <c r="C123" s="49"/>
@@ -4009,10 +4037,10 @@
         <v>8400</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H124" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.45">
@@ -4038,7 +4066,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A126" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B126" s="49"/>
       <c r="C126" s="49"/>
@@ -4067,13 +4095,13 @@
         <v>8002</v>
       </c>
       <c r="G127" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H127" s="47"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A128" s="48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B128" s="48">
         <v>0</v>
@@ -4154,7 +4182,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A135" s="49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B135" s="49"/>
       <c r="C135" s="49"/>
@@ -4198,15 +4226,15 @@
       <c r="E137" s="50"/>
       <c r="F137" s="50"/>
       <c r="G137" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H137" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A138" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B138" s="49"/>
       <c r="C138" s="49"/>
@@ -4254,7 +4282,7 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A141" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B141" s="17"/>
       <c r="C141" s="17"/>
@@ -4278,13 +4306,13 @@
       <c r="E142" s="48"/>
       <c r="F142" s="48"/>
       <c r="G142" s="44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H142" s="47"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A143" s="48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B143" s="48">
         <v>0</v>
@@ -4301,7 +4329,7 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A144" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B144" s="6"/>
       <c r="C144" s="6"/>
@@ -4326,13 +4354,13 @@
       <c r="E145" s="48"/>
       <c r="F145" s="48"/>
       <c r="G145" s="44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H145" s="47"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A146" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B146" s="48">
         <v>1</v>
@@ -4350,7 +4378,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A147" s="49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B147" s="49"/>
       <c r="C147" s="49"/>
@@ -4375,15 +4403,15 @@
       <c r="E148" s="49"/>
       <c r="F148" s="49"/>
       <c r="G148" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H148" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A149" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B149" s="48">
         <v>0</v>
@@ -4400,7 +4428,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A150" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B150" s="49"/>
       <c r="C150" s="49"/>
@@ -4425,13 +4453,13 @@
       <c r="E151" s="49"/>
       <c r="F151" s="49"/>
       <c r="G151" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H151" s="47"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A152" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B152" s="48">
         <v>0</v>
@@ -4459,71 +4487,71 @@
     </row>
     <row r="158" spans="1:8" ht="39.6" x14ac:dyDescent="0.45">
       <c r="A158" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B158" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D158" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E158" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D158" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E158" s="27" t="s">
-        <v>61</v>
-      </c>
       <c r="F158" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A159" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B159" s="17">
         <v>-9</v>
       </c>
       <c r="D159" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E159" s="17">
         <v>4444</v>
       </c>
       <c r="F159" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A160" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B160" s="17">
         <f>B163</f>
         <v>-1</v>
       </c>
       <c r="D160" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E160" s="17">
         <v>5555</v>
       </c>
       <c r="F160" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B161" s="17">
         <v>-2</v>
       </c>
       <c r="D161" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E161" s="17">
         <v>6666</v>
       </c>
       <c r="F161" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.45">
@@ -4534,52 +4562,52 @@
         <v>-2</v>
       </c>
       <c r="D162" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E162" s="17">
         <v>1111</v>
       </c>
       <c r="F162" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B163" s="17">
         <v>-1</v>
       </c>
       <c r="D163" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E163" s="17">
         <v>2222</v>
       </c>
       <c r="F163" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B164" s="17">
         <v>-1</v>
       </c>
       <c r="D164" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E164" s="17">
         <v>3333</v>
       </c>
       <c r="F164" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B165" s="17">
         <v>-1</v>
@@ -4587,7 +4615,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B166" s="17">
         <v>-2</v>
@@ -4595,7 +4623,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B167" s="17">
         <v>-2</v>
@@ -4603,7 +4631,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B168" s="17">
         <v>-9</v>
@@ -4635,7 +4663,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A172" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B172" s="17">
         <v>-1</v>
@@ -4643,7 +4671,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A173" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B173" s="17">
         <v>-1</v>
@@ -4667,7 +4695,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A176" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B176" s="17">
         <v>-2</v>
@@ -4675,7 +4703,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A177" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B177" s="17">
         <v>-2</v>
@@ -4683,7 +4711,7 @@
     </row>
     <row r="180" spans="1:2" ht="249" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed get depallet area by plat is not updated
</commit_message>
<xml_diff>
--- a/testing/デパレ間口_リン.xlsx
+++ b/testing/デパレ間口_リン.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\90181586\Downloads\デパレ間口ソースコード\デパレ間口ソースコード\20251107\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672748BD-EF93-4DCB-9F09-7BD53E01C819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E66BF7-4ACE-4A53-96B1-FB0744126389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="デパレ間口進捗" sheetId="1" r:id="rId1"/>
     <sheet name="デパレ間口の運用" sheetId="2" r:id="rId2"/>
+    <sheet name="API" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="186">
   <si>
     <t>件名</t>
   </si>
@@ -1074,12 +1075,158 @@
     <t xml:space="preserve"> RH3</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>API call</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>payload</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>update_product_info</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://localhost:5000/api/update_product_info</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>②</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>③</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>④</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑤</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑥</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑦</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑧</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑨</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>⑩</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://localhost:5000/api/call_AMR_return</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>call_AMR_return</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>depallet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://localhost:5000/depallet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>query_params</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id=button_id&amp;name=Bライン(L1)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>無し</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:5000/api/line_frontage_click
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://localhost:5000/api/get_depallet_area_by_plat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>get depallet area</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+ "id": button_id
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://localhost:5000/api/update_take_count</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>update_take_count</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{ "maguchi_id": 4, 
+ "kanban_no": "サ607", 
+ "new_take_count": 1
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>display HTML page</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1263,6 +1410,14 @@
       <b/>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -1700,38 +1855,34 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2232,8 +2383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972A1951-796F-43B0-BAF2-5D4B9B88D3C1}">
   <dimension ref="A2:O210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="A157" sqref="A157"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="E180" sqref="E180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -2260,10 +2411,10 @@
       <c r="A4" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="66" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2325,7 +2476,7 @@
       <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="67" t="s">
         <v>127</v>
       </c>
       <c r="B9" s="59"/>
@@ -2339,68 +2490,67 @@
       <c r="J9" s="44"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="57" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="E11" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="F11" s="70"/>
-      <c r="G11" s="76" t="s">
+      <c r="F11" s="69"/>
+      <c r="G11" s="72" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="69">
         <v>2004</v>
       </c>
-      <c r="F12" s="70"/>
-      <c r="G12" s="75">
+      <c r="F12" s="69"/>
+      <c r="G12" s="58">
         <v>1004</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="70"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="75"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
     </row>
     <row r="14" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="62"/>
@@ -2426,7 +2576,7 @@
       <c r="A16" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="49" t="s">
         <v>138</v>
       </c>
       <c r="C16" s="49">
@@ -2450,7 +2600,7 @@
       <c r="A17" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="72">
+      <c r="B17" s="49">
         <v>8504</v>
       </c>
       <c r="C17" s="49">
@@ -2758,37 +2908,35 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="9"/>
-      <c r="H33" s="73"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="H34" s="74"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="66"/>
-      <c r="L34" s="66"/>
-      <c r="M34" s="66"/>
-      <c r="N34" s="66"/>
-      <c r="O34" s="66"/>
+      <c r="H34" s="71"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="76"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="H35" s="74"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="66"/>
-      <c r="O35" s="66"/>
+      <c r="H35" s="71"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="76"/>
+      <c r="L35" s="76"/>
+      <c r="M35" s="76"/>
+      <c r="N35" s="76"/>
+      <c r="O35" s="76"/>
     </row>
     <row r="36" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H36" s="73"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="66"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="66"/>
-      <c r="O36" s="66"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="76"/>
+      <c r="O36" s="76"/>
     </row>
     <row r="37" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
@@ -2809,12 +2957,12 @@
       <c r="F37" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="66"/>
-      <c r="O37" s="66"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="76"/>
+      <c r="O37" s="76"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="52" t="s">
@@ -2835,17 +2983,15 @@
       <c r="F38" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="73"/>
-      <c r="H38" s="73"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="66"/>
-      <c r="L38" s="66"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="66"/>
-      <c r="O38" s="66"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="76"/>
+      <c r="N38" s="76"/>
+      <c r="O38" s="76"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A39" s="68" t="s">
+      <c r="A39" s="67" t="s">
         <v>139</v>
       </c>
       <c r="B39" s="59"/>
@@ -2853,8 +2999,6 @@
       <c r="D39" s="61"/>
       <c r="E39" s="61"/>
       <c r="F39" s="61"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
       <c r="J39" s="60"/>
       <c r="K39" s="60"/>
       <c r="L39" s="60"/>
@@ -2863,16 +3007,14 @@
       <c r="O39" s="60"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A40" s="69" t="s">
+      <c r="A40" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="69"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
+      <c r="F40" s="68"/>
       <c r="J40" s="60"/>
       <c r="K40" s="60"/>
       <c r="L40" s="60"/>
@@ -2881,26 +3023,25 @@
       <c r="O40" s="60"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="70" t="s">
+      <c r="C41" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="70" t="s">
+      <c r="D41" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="70" t="s">
+      <c r="E41" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="F41" s="70"/>
-      <c r="G41" s="76" t="s">
+      <c r="F41" s="69"/>
+      <c r="G41" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="H41" s="73"/>
       <c r="J41" s="60"/>
       <c r="K41" s="60"/>
       <c r="L41" s="60"/>
@@ -2909,26 +3050,25 @@
       <c r="O41" s="60"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A42" s="71" t="s">
+      <c r="A42" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="71" t="s">
+      <c r="C42" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="70" t="s">
+      <c r="D42" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="E42" s="70">
+      <c r="E42" s="69">
         <v>2005</v>
       </c>
-      <c r="F42" s="70"/>
-      <c r="G42" s="73">
+      <c r="F42" s="69"/>
+      <c r="G42" s="7">
         <v>1005</v>
       </c>
-      <c r="H42" s="73"/>
       <c r="J42" s="60"/>
       <c r="K42" s="60"/>
       <c r="L42" s="60"/>
@@ -2937,14 +3077,12 @@
       <c r="O42" s="60"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A43" s="70"/>
-      <c r="B43" s="70"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="73"/>
+      <c r="A43" s="69"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
       <c r="J43" s="60"/>
       <c r="K43" s="60"/>
       <c r="L43" s="60"/>
@@ -2959,8 +3097,6 @@
       <c r="D44" s="62"/>
       <c r="E44" s="62"/>
       <c r="F44" s="62"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
       <c r="J44" s="60"/>
       <c r="K44" s="60"/>
       <c r="L44" s="60"/>
@@ -2977,8 +3113,6 @@
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
       <c r="F45" s="48"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="73"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A46" s="49" t="s">
@@ -2999,8 +3133,6 @@
       <c r="F46" s="49">
         <v>202</v>
       </c>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" s="49" t="s">
@@ -3021,8 +3153,6 @@
       <c r="F47" s="49">
         <v>8500</v>
       </c>
-      <c r="G47" s="73"/>
-      <c r="H47" s="73"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" s="48" t="s">
@@ -3033,8 +3163,6 @@
       <c r="D48" s="48"/>
       <c r="E48" s="48"/>
       <c r="F48" s="48"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="49" t="s">
@@ -3055,8 +3183,6 @@
       <c r="F49" s="49">
         <v>1</v>
       </c>
-      <c r="G49" s="73"/>
-      <c r="H49" s="73"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="49" t="s">
@@ -3077,8 +3203,6 @@
       <c r="F50" s="49">
         <v>8201</v>
       </c>
-      <c r="G50" s="73"/>
-      <c r="H50" s="73"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="48" t="s">
@@ -3399,11 +3523,9 @@
       <c r="F69" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="G69" s="73"/>
-      <c r="H69" s="73"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A70" s="68" t="s">
+      <c r="A70" s="67" t="s">
         <v>143</v>
       </c>
       <c r="B70" s="59"/>
@@ -3411,74 +3533,66 @@
       <c r="D70" s="61"/>
       <c r="E70" s="61"/>
       <c r="F70" s="61"/>
-      <c r="G70" s="73"/>
-      <c r="H70" s="73"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A71" s="69" t="s">
+      <c r="A71" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="69"/>
-      <c r="C71" s="69"/>
-      <c r="D71" s="69"/>
-      <c r="E71" s="69"/>
-      <c r="F71" s="69"/>
-      <c r="G71" s="73"/>
-      <c r="H71" s="73"/>
+      <c r="B71" s="68"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="68"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A72" s="70" t="s">
+      <c r="A72" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="B72" s="70" t="s">
+      <c r="B72" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="70" t="s">
+      <c r="C72" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="D72" s="70" t="s">
+      <c r="D72" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="E72" s="70" t="s">
+      <c r="E72" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="F72" s="70"/>
-      <c r="G72" s="76" t="s">
+      <c r="F72" s="69"/>
+      <c r="G72" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="H72" s="73"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A73" s="71" t="s">
+      <c r="A73" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="B73" s="70" t="s">
+      <c r="B73" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="71" t="s">
+      <c r="C73" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="D73" s="70" t="s">
+      <c r="D73" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="E73" s="70">
+      <c r="E73" s="69">
         <v>2006</v>
       </c>
-      <c r="F73" s="70"/>
-      <c r="G73" s="73">
+      <c r="F73" s="69"/>
+      <c r="G73" s="7">
         <v>1006</v>
       </c>
-      <c r="H73" s="73"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A74" s="70"/>
-      <c r="B74" s="70"/>
-      <c r="C74" s="70"/>
-      <c r="D74" s="70"/>
-      <c r="E74" s="70"/>
-      <c r="F74" s="70"/>
-      <c r="G74" s="73"/>
-      <c r="H74" s="73"/>
+      <c r="A74" s="69"/>
+      <c r="B74" s="69"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="69"/>
+      <c r="F74" s="69"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" s="62"/>
@@ -3487,8 +3601,6 @@
       <c r="D75" s="62"/>
       <c r="E75" s="62"/>
       <c r="F75" s="62"/>
-      <c r="G75" s="73"/>
-      <c r="H75" s="73"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" s="48" t="s">
@@ -3499,8 +3611,6 @@
       <c r="D76" s="48"/>
       <c r="E76" s="48"/>
       <c r="F76" s="48"/>
-      <c r="G76" s="73"/>
-      <c r="H76" s="73"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="49" t="s">
@@ -3517,8 +3627,6 @@
       <c r="F77" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="G77" s="73"/>
-      <c r="H77" s="73"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="49" t="s">
@@ -3535,8 +3643,6 @@
       <c r="F78" s="49">
         <v>8500</v>
       </c>
-      <c r="G78" s="73"/>
-      <c r="H78" s="73"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="48" t="s">
@@ -3547,8 +3653,6 @@
       <c r="D79" s="48"/>
       <c r="E79" s="48"/>
       <c r="F79" s="48"/>
-      <c r="G79" s="73"/>
-      <c r="H79" s="73"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" s="49" t="s">
@@ -3565,8 +3669,6 @@
       <c r="F80" s="49">
         <v>1</v>
       </c>
-      <c r="G80" s="73"/>
-      <c r="H80" s="73"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" s="49" t="s">
@@ -3583,8 +3685,6 @@
       <c r="F81" s="49">
         <v>8200</v>
       </c>
-      <c r="G81" s="73"/>
-      <c r="H81" s="73"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82" s="7" t="s">
@@ -3828,11 +3928,9 @@
       <c r="F98" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="G98" s="73"/>
-      <c r="H98" s="73"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A99" s="68" t="s">
+      <c r="A99" s="67" t="s">
         <v>142</v>
       </c>
       <c r="B99" s="59"/>
@@ -3840,74 +3938,66 @@
       <c r="D99" s="61"/>
       <c r="E99" s="61"/>
       <c r="F99" s="61"/>
-      <c r="G99" s="73"/>
-      <c r="H99" s="73"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A100" s="69" t="s">
+      <c r="A100" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="B100" s="69"/>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
-      <c r="E100" s="69"/>
-      <c r="F100" s="69"/>
-      <c r="G100" s="73"/>
-      <c r="H100" s="73"/>
+      <c r="B100" s="68"/>
+      <c r="C100" s="68"/>
+      <c r="D100" s="68"/>
+      <c r="E100" s="68"/>
+      <c r="F100" s="68"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A101" s="70" t="s">
+      <c r="A101" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="B101" s="70" t="s">
+      <c r="B101" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C101" s="70" t="s">
+      <c r="C101" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="D101" s="70" t="s">
+      <c r="D101" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="E101" s="70" t="s">
+      <c r="E101" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="F101" s="70"/>
-      <c r="G101" s="76" t="s">
+      <c r="F101" s="69"/>
+      <c r="G101" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="H101" s="73"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A102" s="71" t="s">
+      <c r="A102" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="B102" s="70" t="s">
+      <c r="B102" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C102" s="71" t="s">
+      <c r="C102" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="D102" s="70" t="s">
+      <c r="D102" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="E102" s="70">
+      <c r="E102" s="69">
         <v>2001</v>
       </c>
-      <c r="F102" s="70"/>
-      <c r="G102" s="73">
+      <c r="F102" s="69"/>
+      <c r="G102" s="7">
         <v>1001</v>
       </c>
-      <c r="H102" s="73"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A103" s="70"/>
-      <c r="B103" s="70"/>
-      <c r="C103" s="70"/>
-      <c r="D103" s="70"/>
-      <c r="E103" s="70"/>
-      <c r="F103" s="70"/>
-      <c r="G103" s="73"/>
-      <c r="H103" s="73"/>
+      <c r="A103" s="69"/>
+      <c r="B103" s="69"/>
+      <c r="C103" s="69"/>
+      <c r="D103" s="69"/>
+      <c r="E103" s="69"/>
+      <c r="F103" s="69"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A104" s="62"/>
@@ -3916,8 +4006,6 @@
       <c r="D104" s="62"/>
       <c r="E104" s="62"/>
       <c r="F104" s="62"/>
-      <c r="G104" s="73"/>
-      <c r="H104" s="73"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A105" s="48" t="s">
@@ -3928,8 +4016,6 @@
       <c r="D105" s="48"/>
       <c r="E105" s="48"/>
       <c r="F105" s="48"/>
-      <c r="G105" s="73"/>
-      <c r="H105" s="73"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A106" s="49" t="s">
@@ -3950,8 +4036,6 @@
       <c r="F106" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="G106" s="73"/>
-      <c r="H106" s="73"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A107" s="49" t="s">
@@ -3972,8 +4056,6 @@
       <c r="F107" s="49">
         <v>8400</v>
       </c>
-      <c r="G107" s="73"/>
-      <c r="H107" s="73"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A108" s="48" t="s">
@@ -3984,8 +4066,6 @@
       <c r="D108" s="48"/>
       <c r="E108" s="48"/>
       <c r="F108" s="48"/>
-      <c r="G108" s="73"/>
-      <c r="H108" s="73"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A109" s="49" t="s">
@@ -4006,8 +4086,6 @@
       <c r="F109" s="49">
         <v>1</v>
       </c>
-      <c r="G109" s="73"/>
-      <c r="H109" s="73"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A110" s="49" t="s">
@@ -4028,8 +4106,6 @@
       <c r="F110" s="49">
         <v>8000</v>
       </c>
-      <c r="G110" s="73"/>
-      <c r="H110" s="73"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A111" s="17" t="s">
@@ -4322,11 +4398,9 @@
       <c r="F128" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="G128" s="73"/>
-      <c r="H128" s="73"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A129" s="68" t="s">
+      <c r="A129" s="67" t="s">
         <v>142</v>
       </c>
       <c r="B129" s="59"/>
@@ -4334,74 +4408,66 @@
       <c r="D129" s="61"/>
       <c r="E129" s="61"/>
       <c r="F129" s="61"/>
-      <c r="G129" s="73"/>
-      <c r="H129" s="73"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A130" s="69" t="s">
+      <c r="A130" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="B130" s="69"/>
-      <c r="C130" s="69"/>
-      <c r="D130" s="69"/>
-      <c r="E130" s="69"/>
-      <c r="F130" s="69"/>
-      <c r="G130" s="73"/>
-      <c r="H130" s="73"/>
+      <c r="B130" s="68"/>
+      <c r="C130" s="68"/>
+      <c r="D130" s="68"/>
+      <c r="E130" s="68"/>
+      <c r="F130" s="68"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A131" s="70" t="s">
+      <c r="A131" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="B131" s="70" t="s">
+      <c r="B131" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C131" s="70" t="s">
+      <c r="C131" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="D131" s="70" t="s">
+      <c r="D131" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="E131" s="70" t="s">
+      <c r="E131" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="F131" s="70"/>
-      <c r="G131" s="76" t="s">
+      <c r="F131" s="69"/>
+      <c r="G131" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="H131" s="73"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A132" s="71" t="s">
+      <c r="A132" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="B132" s="70" t="s">
+      <c r="B132" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C132" s="71" t="s">
+      <c r="C132" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="D132" s="70" t="s">
+      <c r="D132" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="E132" s="70">
+      <c r="E132" s="69">
         <v>2002</v>
       </c>
-      <c r="F132" s="70"/>
-      <c r="G132" s="73">
+      <c r="F132" s="69"/>
+      <c r="G132" s="7">
         <v>1002</v>
       </c>
-      <c r="H132" s="73"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A133" s="70"/>
-      <c r="B133" s="70"/>
-      <c r="C133" s="70"/>
-      <c r="D133" s="70"/>
-      <c r="E133" s="70"/>
-      <c r="F133" s="70"/>
-      <c r="G133" s="73"/>
-      <c r="H133" s="73"/>
+      <c r="A133" s="69"/>
+      <c r="B133" s="69"/>
+      <c r="C133" s="69"/>
+      <c r="D133" s="69"/>
+      <c r="E133" s="69"/>
+      <c r="F133" s="69"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A134" s="62"/>
@@ -4410,8 +4476,6 @@
       <c r="D134" s="62"/>
       <c r="E134" s="62"/>
       <c r="F134" s="62"/>
-      <c r="G134" s="73"/>
-      <c r="H134" s="73"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A135" s="48" t="s">
@@ -4422,8 +4486,6 @@
       <c r="D135" s="48"/>
       <c r="E135" s="48"/>
       <c r="F135" s="48"/>
-      <c r="G135" s="73"/>
-      <c r="H135" s="73"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A136" s="49" t="s">
@@ -4444,8 +4506,6 @@
       <c r="F136" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="G136" s="73"/>
-      <c r="H136" s="73"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A137" s="49" t="s">
@@ -4466,8 +4526,6 @@
       <c r="F137" s="49">
         <v>8400</v>
       </c>
-      <c r="G137" s="73"/>
-      <c r="H137" s="73"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A138" s="48" t="s">
@@ -4478,8 +4536,6 @@
       <c r="D138" s="48"/>
       <c r="E138" s="48"/>
       <c r="F138" s="48"/>
-      <c r="G138" s="73"/>
-      <c r="H138" s="73"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A139" s="49" t="s">
@@ -4500,8 +4556,6 @@
       <c r="F139" s="49">
         <v>1</v>
       </c>
-      <c r="G139" s="73"/>
-      <c r="H139" s="73"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A140" s="49" t="s">
@@ -4514,7 +4568,7 @@
         <v>8046</v>
       </c>
       <c r="D140" s="49">
-        <v>8032</v>
+        <v>8031</v>
       </c>
       <c r="E140" s="49">
         <v>8016</v>
@@ -4522,8 +4576,6 @@
       <c r="F140" s="49">
         <v>8000</v>
       </c>
-      <c r="G140" s="73"/>
-      <c r="H140" s="73"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A141" s="17" t="s">
@@ -4546,7 +4598,7 @@
         <v>8046</v>
       </c>
       <c r="D142" s="47">
-        <v>8032</v>
+        <v>8031</v>
       </c>
       <c r="E142" s="47">
         <v>8016</v>
@@ -4808,11 +4860,9 @@
       <c r="F158" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="G158" s="73"/>
-      <c r="H158" s="73"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A159" s="68" t="s">
+      <c r="A159" s="67" t="s">
         <v>142</v>
       </c>
       <c r="B159" s="59"/>
@@ -4820,74 +4870,66 @@
       <c r="D159" s="61"/>
       <c r="E159" s="61"/>
       <c r="F159" s="61"/>
-      <c r="G159" s="73"/>
-      <c r="H159" s="73"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A160" s="69" t="s">
+      <c r="A160" s="68" t="s">
         <v>144</v>
       </c>
-      <c r="B160" s="69"/>
-      <c r="C160" s="69"/>
-      <c r="D160" s="69"/>
-      <c r="E160" s="69"/>
-      <c r="F160" s="69"/>
-      <c r="G160" s="73"/>
-      <c r="H160" s="73"/>
+      <c r="B160" s="68"/>
+      <c r="C160" s="68"/>
+      <c r="D160" s="68"/>
+      <c r="E160" s="68"/>
+      <c r="F160" s="68"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A161" s="70" t="s">
+      <c r="A161" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="B161" s="70" t="s">
+      <c r="B161" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="C161" s="70" t="s">
+      <c r="C161" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="D161" s="70" t="s">
+      <c r="D161" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="E161" s="70" t="s">
+      <c r="E161" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="F161" s="70"/>
-      <c r="G161" s="76" t="s">
+      <c r="F161" s="69"/>
+      <c r="G161" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="H161" s="73"/>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A162" s="71" t="s">
+      <c r="A162" s="70" t="s">
         <v>129</v>
       </c>
-      <c r="B162" s="70" t="s">
+      <c r="B162" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="C162" s="71" t="s">
+      <c r="C162" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="D162" s="70" t="s">
+      <c r="D162" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="E162" s="70">
+      <c r="E162" s="69">
         <v>2003</v>
       </c>
-      <c r="F162" s="70"/>
-      <c r="G162" s="73">
+      <c r="F162" s="69"/>
+      <c r="G162" s="7">
         <v>1003</v>
       </c>
-      <c r="H162" s="73"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A163" s="70"/>
-      <c r="B163" s="70"/>
-      <c r="C163" s="70"/>
-      <c r="D163" s="70"/>
-      <c r="E163" s="70"/>
-      <c r="F163" s="70"/>
-      <c r="G163" s="73"/>
-      <c r="H163" s="73"/>
+      <c r="A163" s="69"/>
+      <c r="B163" s="69"/>
+      <c r="C163" s="69"/>
+      <c r="D163" s="69"/>
+      <c r="E163" s="69"/>
+      <c r="F163" s="69"/>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A164" s="62"/>
@@ -4896,8 +4938,6 @@
       <c r="D164" s="62"/>
       <c r="E164" s="62"/>
       <c r="F164" s="62"/>
-      <c r="G164" s="73"/>
-      <c r="H164" s="73"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A165" s="48" t="s">
@@ -4908,8 +4948,6 @@
       <c r="D165" s="48"/>
       <c r="E165" s="48"/>
       <c r="F165" s="48"/>
-      <c r="G165" s="73"/>
-      <c r="H165" s="73"/>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A166" s="49" t="s">
@@ -4926,8 +4964,6 @@
       </c>
       <c r="E166" s="49"/>
       <c r="F166" s="49"/>
-      <c r="G166" s="73"/>
-      <c r="H166" s="73"/>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A167" s="49" t="s">
@@ -4944,8 +4980,6 @@
       </c>
       <c r="E167" s="49"/>
       <c r="F167" s="49"/>
-      <c r="G167" s="73"/>
-      <c r="H167" s="73"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A168" s="48" t="s">
@@ -4956,8 +4990,6 @@
       <c r="D168" s="48"/>
       <c r="E168" s="48"/>
       <c r="F168" s="48"/>
-      <c r="G168" s="73"/>
-      <c r="H168" s="73"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A169" s="49" t="s">
@@ -4974,8 +5006,6 @@
       </c>
       <c r="E169" s="49"/>
       <c r="F169" s="49"/>
-      <c r="G169" s="73"/>
-      <c r="H169" s="73"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A170" s="49" t="s">
@@ -4988,12 +5018,10 @@
         <v>8046</v>
       </c>
       <c r="D170" s="49">
-        <v>8032</v>
+        <v>8031</v>
       </c>
       <c r="E170" s="49"/>
       <c r="F170" s="49"/>
-      <c r="G170" s="73"/>
-      <c r="H170" s="73"/>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A171" s="17" t="s">
@@ -5016,7 +5044,7 @@
         <v>8046</v>
       </c>
       <c r="D172" s="47">
-        <v>8032</v>
+        <v>8031</v>
       </c>
       <c r="E172" s="47"/>
       <c r="F172" s="47"/>
@@ -5437,4 +5465,187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4385DC4-C887-4AF3-BCD1-3446DCE3B983}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="19.09765625" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="33.69921875" customWidth="1"/>
+    <col min="6" max="6" width="40.296875" customWidth="1"/>
+    <col min="7" max="7" width="41.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="73" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="54" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{D9200F41-5AE1-455C-8735-FECEC0823D12}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{D54D4065-7478-43CE-8ECA-36993D68834F}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{E4EFC330-8AE4-4955-92DF-09D3914DD417}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{59573920-1777-4285-9419-6143F7DD47FD}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{B0E65741-1039-4E29-9FDE-7366C9A011A3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the config cannot update issue for get depallet by plat
</commit_message>
<xml_diff>
--- a/testing/デパレ間口_リン.xlsx
+++ b/testing/デパレ間口_リン.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\90181586\Downloads\知立工場開発\depare_maguchi\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB6473D-AA59-420E-A95D-DBCE53D094E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10988E09-176A-4C6C-ACAC-0141E1C3F65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="21636" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="残課題進捗" sheetId="1" r:id="rId1"/>
+    <sheet name="残課題修正" sheetId="1" r:id="rId1"/>
     <sheet name="進捗" sheetId="4" r:id="rId2"/>
     <sheet name="基本設計書" sheetId="5" r:id="rId3"/>
     <sheet name="デパレ運用トライ" sheetId="2" r:id="rId4"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="284">
   <si>
     <t>line_inventory テーブル</t>
   </si>
@@ -2443,6 +2443,21 @@
       </rPr>
       <t>@app.route("/b_line_depallet_maguchi", methods=["GET"])</t>
     </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エラーメッセージ handling for take_count api</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>完了</t>
+    <rPh sb="0" eb="2">
+      <t>カンリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pause setInterval in frontend and reload config in get depallet_area_by_id API</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3147,7 +3162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3347,24 +3362,6 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3374,9 +3371,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3392,16 +3386,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="56" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -3415,33 +3400,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -3460,26 +3418,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3818,8 +3824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -3831,20 +3837,20 @@
     <col min="5" max="5" width="51.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="77" customFormat="1" ht="31.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="77" t="s" ph="1">
+    <row r="1" spans="1:5" s="71" customFormat="1" ht="31.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="71" t="s" ph="1">
         <v>154</v>
       </c>
-      <c r="B1" s="77" t="s" ph="1">
+      <c r="B1" s="71" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="C1" s="77" t="s" ph="1">
+      <c r="C1" s="71" t="s" ph="1">
         <v>89</v>
       </c>
-      <c r="D1" s="77" t="s" ph="1">
+      <c r="D1" s="71" t="s" ph="1">
         <v>6</v>
       </c>
-      <c r="E1" s="77" t="s" ph="1">
+      <c r="E1" s="71" t="s" ph="1">
         <v>4</v>
       </c>
     </row>
@@ -3958,7 +3964,19 @@
         <v>182</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>164</v>
+        <v>282</v>
+      </c>
+      <c r="D11" s="99" t="s">
+        <v>283</v>
+      </c>
+      <c r="E11" s="99"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -3983,6 +4001,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D11:E11"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{AD0AC432-884C-47C5-A353-DF628881C76E}"/>
@@ -4023,7 +4044,7 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" s="87">
+      <c r="A7" s="79">
         <v>45964</v>
       </c>
     </row>
@@ -4033,7 +4054,7 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" s="87">
+      <c r="A10" s="79">
         <v>45965</v>
       </c>
     </row>
@@ -4102,35 +4123,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4755DEB-EA68-4311-AA25-1884341C82CB}">
   <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H6" sqref="H6:Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="107" t="s">
         <v>278</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -4139,124 +4160,124 @@
     </row>
     <row r="4" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="108" t="s">
         <v>227</v>
       </c>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96" t="s">
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109" t="s">
         <v>228</v>
       </c>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="96"/>
-      <c r="T5" s="96"/>
-      <c r="U5" s="96"/>
-      <c r="V5" s="96"/>
-      <c r="W5" s="96"/>
-      <c r="X5" s="96"/>
-      <c r="Y5" s="97"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="109"/>
+      <c r="N5" s="109"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="109"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="110"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A6" s="98"/>
-      <c r="B6" s="99"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
-      <c r="H6" s="99" t="s">
+      <c r="A6" s="105"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103" t="s">
         <v>229</v>
       </c>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
-      <c r="N6" s="99"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="99"/>
-      <c r="S6" s="99"/>
-      <c r="T6" s="99"/>
-      <c r="U6" s="99"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="99"/>
-      <c r="X6" s="99"/>
-      <c r="Y6" s="100"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="103"/>
+      <c r="S6" s="103"/>
+      <c r="T6" s="103"/>
+      <c r="U6" s="103"/>
+      <c r="V6" s="103"/>
+      <c r="W6" s="103"/>
+      <c r="X6" s="103"/>
+      <c r="Y6" s="104"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A7" s="98"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="99"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="99"/>
-      <c r="U7" s="99"/>
-      <c r="V7" s="99"/>
-      <c r="W7" s="99"/>
-      <c r="X7" s="99"/>
-      <c r="Y7" s="100"/>
+      <c r="A7" s="105"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="103"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="103"/>
+      <c r="S7" s="103"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="103"/>
+      <c r="V7" s="103"/>
+      <c r="W7" s="103"/>
+      <c r="X7" s="103"/>
+      <c r="Y7" s="104"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="105" t="s">
         <v>230</v>
       </c>
-      <c r="B8" s="99"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99" t="s">
+      <c r="B8" s="103"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103" t="s">
         <v>231</v>
       </c>
-      <c r="H8" s="99"/>
-      <c r="I8" s="99"/>
-      <c r="J8" s="99"/>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
-      <c r="N8" s="99" t="s">
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103" t="s">
         <v>232</v>
       </c>
-      <c r="O8" s="99"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="99"/>
-      <c r="S8" s="99"/>
-      <c r="T8" s="99"/>
-      <c r="U8" s="99"/>
-      <c r="V8" s="99"/>
-      <c r="W8" s="99"/>
-      <c r="X8" s="99"/>
-      <c r="Y8" s="100"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="103"/>
+      <c r="U8" s="103"/>
+      <c r="V8" s="103"/>
+      <c r="W8" s="103"/>
+      <c r="X8" s="103"/>
+      <c r="Y8" s="104"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="101" t="s">
@@ -4267,25 +4288,25 @@
       <c r="D9" s="102"/>
       <c r="E9" s="102"/>
       <c r="F9" s="102"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="99"/>
-      <c r="M9" s="99"/>
-      <c r="N9" s="99"/>
-      <c r="O9" s="99"/>
-      <c r="P9" s="99"/>
-      <c r="Q9" s="99"/>
-      <c r="R9" s="99"/>
-      <c r="S9" s="99"/>
-      <c r="T9" s="99"/>
-      <c r="U9" s="99"/>
-      <c r="V9" s="99"/>
-      <c r="W9" s="99"/>
-      <c r="X9" s="99"/>
-      <c r="Y9" s="100"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="103"/>
+      <c r="N9" s="103"/>
+      <c r="O9" s="103"/>
+      <c r="P9" s="103"/>
+      <c r="Q9" s="103"/>
+      <c r="R9" s="103"/>
+      <c r="S9" s="103"/>
+      <c r="T9" s="103"/>
+      <c r="U9" s="103"/>
+      <c r="V9" s="103"/>
+      <c r="W9" s="103"/>
+      <c r="X9" s="103"/>
+      <c r="Y9" s="104"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="101"/>
@@ -4294,404 +4315,412 @@
       <c r="D10" s="102"/>
       <c r="E10" s="102"/>
       <c r="F10" s="102"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="99"/>
-      <c r="N10" s="99"/>
-      <c r="O10" s="99"/>
-      <c r="P10" s="99"/>
-      <c r="Q10" s="99"/>
-      <c r="R10" s="99"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="99"/>
-      <c r="U10" s="99"/>
-      <c r="V10" s="99"/>
-      <c r="W10" s="99"/>
-      <c r="X10" s="99"/>
-      <c r="Y10" s="100"/>
+      <c r="G10" s="103"/>
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="103"/>
+      <c r="K10" s="103"/>
+      <c r="L10" s="103"/>
+      <c r="M10" s="103"/>
+      <c r="N10" s="103"/>
+      <c r="O10" s="103"/>
+      <c r="P10" s="103"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="103"/>
+      <c r="S10" s="103"/>
+      <c r="T10" s="103"/>
+      <c r="U10" s="103"/>
+      <c r="V10" s="103"/>
+      <c r="W10" s="103"/>
+      <c r="X10" s="103"/>
+      <c r="Y10" s="104"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="105" t="s">
         <v>234</v>
       </c>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="99" t="s">
+      <c r="B11" s="103"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="103"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="103"/>
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="J11" s="103"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="106"/>
+      <c r="M11" s="103" t="s">
         <v>235</v>
       </c>
-      <c r="N11" s="99"/>
-      <c r="O11" s="99"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="99"/>
-      <c r="R11" s="99"/>
-      <c r="S11" s="99"/>
-      <c r="T11" s="99"/>
-      <c r="U11" s="99"/>
-      <c r="V11" s="99"/>
-      <c r="W11" s="99"/>
-      <c r="X11" s="99"/>
-      <c r="Y11" s="100"/>
+      <c r="N11" s="103"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="103"/>
+      <c r="S11" s="103"/>
+      <c r="T11" s="103"/>
+      <c r="U11" s="103"/>
+      <c r="V11" s="103"/>
+      <c r="W11" s="103"/>
+      <c r="X11" s="103"/>
+      <c r="Y11" s="104"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A12" s="115" t="s">
+      <c r="A12" s="95" t="s">
         <v>279</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
-      <c r="L12" s="117"/>
-      <c r="M12" s="105"/>
-      <c r="Y12" s="106"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="97"/>
+      <c r="M12" s="86"/>
+      <c r="Y12" s="87"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A13" s="120" t="s">
+      <c r="A13" s="98" t="s">
         <v>280</v>
       </c>
-      <c r="B13" s="118"/>
-      <c r="C13" s="118"/>
-      <c r="D13" s="118"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
-      <c r="J13" s="118"/>
-      <c r="K13" s="118"/>
-      <c r="L13" s="119"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="108" t="s">
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="99"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="89" t="s">
         <v>236</v>
       </c>
-      <c r="Y13" s="106"/>
+      <c r="Y13" s="87"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A14" s="104"/>
-      <c r="B14" s="107"/>
-      <c r="M14" s="105"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="88"/>
+      <c r="M14" s="86"/>
       <c r="N14" t="s">
         <v>237</v>
       </c>
-      <c r="Y14" s="106"/>
+      <c r="Y14" s="87"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A15" s="104"/>
-      <c r="B15" s="107" t="s">
+      <c r="A15" s="85"/>
+      <c r="B15" s="88" t="s">
         <v>238</v>
       </c>
-      <c r="M15" s="105"/>
+      <c r="M15" s="86"/>
       <c r="N15" t="s">
         <v>239</v>
       </c>
-      <c r="Y15" s="106"/>
+      <c r="Y15" s="87"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A16" s="104"/>
-      <c r="B16" s="107" t="s">
+      <c r="A16" s="85"/>
+      <c r="B16" s="88" t="s">
         <v>240</v>
       </c>
-      <c r="M16" s="105"/>
+      <c r="M16" s="86"/>
       <c r="N16" t="s">
         <v>241</v>
       </c>
-      <c r="Y16" s="106"/>
+      <c r="Y16" s="87"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A17" s="104"/>
-      <c r="B17" s="107" t="s">
+      <c r="A17" s="85"/>
+      <c r="B17" s="88" t="s">
         <v>242</v>
       </c>
-      <c r="M17" s="105"/>
+      <c r="M17" s="86"/>
       <c r="N17" t="s">
         <v>243</v>
       </c>
-      <c r="Y17" s="106"/>
+      <c r="Y17" s="87"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A18" s="104"/>
-      <c r="B18" s="107" t="s">
+      <c r="A18" s="85"/>
+      <c r="B18" s="88" t="s">
         <v>244</v>
       </c>
-      <c r="M18" s="105"/>
+      <c r="M18" s="86"/>
       <c r="N18" t="s">
         <v>245</v>
       </c>
-      <c r="Y18" s="106"/>
+      <c r="Y18" s="87"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A19" s="104"/>
-      <c r="B19" s="107" t="s">
+      <c r="A19" s="85"/>
+      <c r="B19" s="88" t="s">
         <v>246</v>
       </c>
-      <c r="M19" s="105"/>
+      <c r="M19" s="86"/>
       <c r="N19" t="s">
         <v>247</v>
       </c>
-      <c r="Y19" s="106"/>
+      <c r="Y19" s="87"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A20" s="104"/>
-      <c r="B20" s="107" t="s">
+      <c r="A20" s="85"/>
+      <c r="B20" s="88" t="s">
         <v>248</v>
       </c>
-      <c r="M20" s="105"/>
+      <c r="M20" s="86"/>
       <c r="N20" t="s">
         <v>249</v>
       </c>
-      <c r="Y20" s="106"/>
+      <c r="Y20" s="87"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A21" s="104"/>
-      <c r="C21" s="109" t="s">
+      <c r="A21" s="85"/>
+      <c r="C21" s="90" t="s">
         <v>250</v>
       </c>
-      <c r="M21" s="105"/>
+      <c r="M21" s="86"/>
       <c r="O21" t="s">
         <v>251</v>
       </c>
-      <c r="Y21" s="106"/>
+      <c r="Y21" s="87"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A22" s="104"/>
-      <c r="C22" s="109" t="s">
+      <c r="A22" s="85"/>
+      <c r="C22" s="90" t="s">
         <v>252</v>
       </c>
-      <c r="M22" s="105"/>
+      <c r="M22" s="86"/>
       <c r="O22" t="s">
         <v>253</v>
       </c>
-      <c r="Y22" s="106"/>
+      <c r="Y22" s="87"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A23" s="104"/>
-      <c r="B23" s="107" t="s">
+      <c r="A23" s="85"/>
+      <c r="B23" s="88" t="s">
         <v>254</v>
       </c>
-      <c r="M23" s="105"/>
+      <c r="M23" s="86"/>
       <c r="N23" t="s">
         <v>255</v>
       </c>
-      <c r="Y23" s="106"/>
+      <c r="Y23" s="87"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A24" s="104"/>
-      <c r="B24" s="107" t="s">
+      <c r="A24" s="85"/>
+      <c r="B24" s="88" t="s">
         <v>256</v>
       </c>
-      <c r="M24" s="105"/>
+      <c r="M24" s="86"/>
       <c r="N24" t="s">
         <v>257</v>
       </c>
-      <c r="Y24" s="106"/>
+      <c r="Y24" s="87"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A25" s="104"/>
-      <c r="B25" s="107" t="s">
+      <c r="A25" s="85"/>
+      <c r="B25" s="88" t="s">
         <v>258</v>
       </c>
-      <c r="M25" s="105"/>
+      <c r="M25" s="86"/>
       <c r="N25" t="s">
         <v>259</v>
       </c>
-      <c r="Y25" s="106"/>
+      <c r="Y25" s="87"/>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A26" s="104"/>
-      <c r="B26" s="107" t="s">
+      <c r="A26" s="85"/>
+      <c r="B26" s="88" t="s">
         <v>260</v>
       </c>
-      <c r="M26" s="105"/>
+      <c r="M26" s="86"/>
       <c r="N26" t="s">
         <v>261</v>
       </c>
-      <c r="Y26" s="106"/>
+      <c r="Y26" s="87"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A27" s="104"/>
-      <c r="B27" s="107" t="s">
+      <c r="A27" s="85"/>
+      <c r="B27" s="88" t="s">
         <v>262</v>
       </c>
-      <c r="M27" s="105"/>
+      <c r="M27" s="86"/>
       <c r="N27" t="s">
         <v>263</v>
       </c>
-      <c r="Y27" s="106"/>
+      <c r="Y27" s="87"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A28" s="104"/>
-      <c r="B28" s="107" t="s">
+      <c r="A28" s="85"/>
+      <c r="B28" s="88" t="s">
         <v>264</v>
       </c>
-      <c r="M28" s="105"/>
+      <c r="M28" s="86"/>
       <c r="N28" t="s">
         <v>265</v>
       </c>
-      <c r="Y28" s="106"/>
+      <c r="Y28" s="87"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A29" s="104"/>
-      <c r="B29" s="107" t="s">
+      <c r="A29" s="85"/>
+      <c r="B29" s="88" t="s">
         <v>266</v>
       </c>
-      <c r="M29" s="105"/>
+      <c r="M29" s="86"/>
       <c r="N29" t="s">
         <v>267</v>
       </c>
-      <c r="Y29" s="106"/>
+      <c r="Y29" s="87"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A30" s="104"/>
-      <c r="B30" s="107" t="s">
+      <c r="A30" s="85"/>
+      <c r="B30" s="88" t="s">
         <v>268</v>
       </c>
-      <c r="M30" s="105"/>
+      <c r="M30" s="86"/>
       <c r="N30" t="s">
         <v>269</v>
       </c>
-      <c r="Y30" s="106"/>
+      <c r="Y30" s="87"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A31" s="104"/>
-      <c r="B31" s="107" t="s">
+      <c r="A31" s="85"/>
+      <c r="B31" s="88" t="s">
         <v>270</v>
       </c>
-      <c r="M31" s="105"/>
+      <c r="M31" s="86"/>
       <c r="N31" t="s">
         <v>271</v>
       </c>
-      <c r="Y31" s="106"/>
+      <c r="Y31" s="87"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A32" s="104"/>
-      <c r="B32" s="107" t="s">
+      <c r="A32" s="85"/>
+      <c r="B32" s="88" t="s">
         <v>272</v>
       </c>
-      <c r="M32" s="105"/>
+      <c r="M32" s="86"/>
       <c r="N32" t="s">
         <v>273</v>
       </c>
-      <c r="Y32" s="106"/>
+      <c r="Y32" s="87"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A33" s="104"/>
-      <c r="B33" s="107" t="s">
+      <c r="A33" s="85"/>
+      <c r="B33" s="88" t="s">
         <v>274</v>
       </c>
-      <c r="M33" s="105"/>
+      <c r="M33" s="86"/>
       <c r="N33" t="s">
         <v>275</v>
       </c>
-      <c r="Y33" s="106"/>
+      <c r="Y33" s="87"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A34" s="104"/>
-      <c r="B34" s="107" t="s">
+      <c r="A34" s="85"/>
+      <c r="B34" s="88" t="s">
         <v>276</v>
       </c>
-      <c r="M34" s="105"/>
+      <c r="M34" s="86"/>
       <c r="N34" t="s">
         <v>277</v>
       </c>
-      <c r="Y34" s="106"/>
+      <c r="Y34" s="87"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A35" s="104"/>
-      <c r="M35" s="105"/>
-      <c r="Y35" s="106"/>
+      <c r="A35" s="85"/>
+      <c r="M35" s="86"/>
+      <c r="Y35" s="87"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A36" s="104"/>
-      <c r="M36" s="105"/>
-      <c r="Y36" s="106"/>
+      <c r="A36" s="85"/>
+      <c r="M36" s="86"/>
+      <c r="Y36" s="87"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A37" s="104"/>
-      <c r="M37" s="105"/>
-      <c r="Y37" s="106"/>
+      <c r="A37" s="85"/>
+      <c r="M37" s="86"/>
+      <c r="Y37" s="87"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A38" s="104"/>
-      <c r="M38" s="105"/>
-      <c r="Y38" s="106"/>
+      <c r="A38" s="85"/>
+      <c r="M38" s="86"/>
+      <c r="Y38" s="87"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A39" s="104"/>
-      <c r="M39" s="105"/>
-      <c r="Y39" s="106"/>
+      <c r="A39" s="85"/>
+      <c r="M39" s="86"/>
+      <c r="Y39" s="87"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A40" s="104"/>
-      <c r="M40" s="105"/>
-      <c r="Y40" s="106"/>
+      <c r="A40" s="85"/>
+      <c r="M40" s="86"/>
+      <c r="Y40" s="87"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A41" s="104"/>
-      <c r="M41" s="105"/>
-      <c r="Y41" s="106"/>
+      <c r="A41" s="85"/>
+      <c r="M41" s="86"/>
+      <c r="Y41" s="87"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A42" s="104"/>
-      <c r="M42" s="105"/>
-      <c r="Y42" s="106"/>
+      <c r="A42" s="85"/>
+      <c r="M42" s="86"/>
+      <c r="Y42" s="87"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A43" s="104"/>
-      <c r="M43" s="105"/>
-      <c r="Y43" s="106"/>
+      <c r="A43" s="85"/>
+      <c r="M43" s="86"/>
+      <c r="Y43" s="87"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A44" s="104"/>
-      <c r="M44" s="105"/>
-      <c r="Y44" s="106"/>
+      <c r="A44" s="85"/>
+      <c r="M44" s="86"/>
+      <c r="Y44" s="87"/>
     </row>
     <row r="45" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="110"/>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="111"/>
-      <c r="J45" s="111"/>
-      <c r="K45" s="111"/>
-      <c r="L45" s="111"/>
-      <c r="M45" s="112"/>
-      <c r="N45" s="111"/>
-      <c r="O45" s="111"/>
-      <c r="P45" s="111"/>
-      <c r="Q45" s="111"/>
-      <c r="R45" s="111"/>
-      <c r="S45" s="111"/>
-      <c r="T45" s="111"/>
-      <c r="U45" s="111"/>
-      <c r="V45" s="111"/>
-      <c r="W45" s="111"/>
-      <c r="X45" s="111"/>
-      <c r="Y45" s="113"/>
+      <c r="A45" s="91"/>
+      <c r="B45" s="92"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="92"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="92"/>
+      <c r="L45" s="92"/>
+      <c r="M45" s="93"/>
+      <c r="N45" s="92"/>
+      <c r="O45" s="92"/>
+      <c r="P45" s="92"/>
+      <c r="Q45" s="92"/>
+      <c r="R45" s="92"/>
+      <c r="S45" s="92"/>
+      <c r="T45" s="92"/>
+      <c r="U45" s="92"/>
+      <c r="V45" s="92"/>
+      <c r="W45" s="92"/>
+      <c r="X45" s="92"/>
+      <c r="Y45" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="G8:M8"/>
+    <mergeCell ref="N8:Y8"/>
+    <mergeCell ref="E1:M2"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="H5:Y5"/>
+    <mergeCell ref="A6:G7"/>
+    <mergeCell ref="H6:Y7"/>
     <mergeCell ref="A12:L12"/>
     <mergeCell ref="A13:L13"/>
     <mergeCell ref="A9:F10"/>
@@ -4699,14 +4728,6 @@
     <mergeCell ref="N9:Y10"/>
     <mergeCell ref="A11:L11"/>
     <mergeCell ref="M11:Y11"/>
-    <mergeCell ref="E1:M2"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="H5:Y5"/>
-    <mergeCell ref="A6:G7"/>
-    <mergeCell ref="H6:Y7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="G8:M8"/>
-    <mergeCell ref="N8:Y8"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4740,42 +4761,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="114" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
     </row>
     <row r="5" spans="2:14" ht="28.8" x14ac:dyDescent="0.45">
       <c r="B5" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="116" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
     </row>
     <row r="6" spans="2:14" ht="28.8" x14ac:dyDescent="0.45">
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
     </row>
     <row r="7" spans="2:14" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B7" s="5" t="s">
@@ -4841,10 +4862,10 @@
       <c r="G10" s="43"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="117" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="76"/>
+      <c r="C11" s="117"/>
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
       <c r="F11" s="68"/>
@@ -4873,22 +4894,22 @@
       </c>
     </row>
     <row r="13" spans="2:14" s="50" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="90" t="s">
+      <c r="B13" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="C13" s="90" t="s">
+      <c r="C13" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="90" t="s">
+      <c r="D13" s="80" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="90" t="s">
+      <c r="E13" s="80" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="90" t="s">
+      <c r="F13" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="90"/>
+      <c r="G13" s="80"/>
       <c r="H13" s="55" t="s">
         <v>126</v>
       </c>
@@ -4900,22 +4921,22 @@
       </c>
     </row>
     <row r="14" spans="2:14" s="50" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="80" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="80" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="90" t="s">
+      <c r="D14" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="90" t="s">
+      <c r="E14" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="F14" s="90">
+      <c r="F14" s="80">
         <v>2004</v>
       </c>
-      <c r="G14" s="90"/>
+      <c r="G14" s="80"/>
       <c r="H14" s="50">
         <v>1004</v>
       </c>
@@ -5121,7 +5142,7 @@
       <c r="G24" s="42">
         <v>0</v>
       </c>
-      <c r="I24" s="93"/>
+      <c r="I24" s="83"/>
       <c r="M24" s="15" t="s">
         <v>45</v>
       </c>
@@ -5151,7 +5172,7 @@
       <c r="H25" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I25" s="93"/>
+      <c r="I25" s="83"/>
       <c r="M25" s="15">
         <v>3238</v>
       </c>
@@ -5169,7 +5190,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="93"/>
+      <c r="I26" s="83"/>
       <c r="M26" s="15" t="s">
         <v>67</v>
       </c>
@@ -5196,7 +5217,7 @@
       <c r="G27" s="42">
         <v>1</v>
       </c>
-      <c r="I27" s="93"/>
+      <c r="I27" s="83"/>
       <c r="M27" s="15" t="s">
         <v>68</v>
       </c>
@@ -5226,7 +5247,7 @@
       <c r="H28" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I28" s="93"/>
+      <c r="I28" s="83"/>
       <c r="M28" s="15" t="s">
         <v>35</v>
       </c>
@@ -5243,7 +5264,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
-      <c r="I29" s="93"/>
+      <c r="I29" s="83"/>
       <c r="M29" s="15" t="s">
         <v>46</v>
       </c>
@@ -5270,7 +5291,7 @@
       <c r="G30" s="42">
         <v>0</v>
       </c>
-      <c r="I30" s="93" t="s">
+      <c r="I30" s="83" t="s">
         <v>88</v>
       </c>
       <c r="M30" s="15" t="s">
@@ -5302,7 +5323,7 @@
       <c r="H31" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I31" s="93"/>
+      <c r="I31" s="83"/>
       <c r="M31" s="15" t="s">
         <v>70</v>
       </c>
@@ -5319,7 +5340,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="I32" s="93"/>
+      <c r="I32" s="83"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B33" s="42" t="s">
@@ -5340,7 +5361,7 @@
       <c r="G33" s="42">
         <v>0</v>
       </c>
-      <c r="I33" s="93"/>
+      <c r="I33" s="83"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B34" s="42" t="s">
@@ -5364,7 +5385,7 @@
       <c r="H34" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I34" s="93"/>
+      <c r="I34" s="83"/>
       <c r="M34" s="20"/>
     </row>
     <row r="35" spans="2:15" ht="23.4" customHeight="1" x14ac:dyDescent="0.45">
@@ -5376,7 +5397,7 @@
       <c r="E35" s="60"/>
       <c r="F35" s="60"/>
       <c r="G35" s="60"/>
-      <c r="I35" s="93"/>
+      <c r="I35" s="83"/>
       <c r="M35" s="21" t="s">
         <v>73</v>
       </c>
@@ -5484,10 +5505,10 @@
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="111" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="72"/>
+      <c r="C41" s="112"/>
       <c r="D41" s="51"/>
       <c r="E41" s="51"/>
       <c r="F41" s="51"/>
@@ -5503,64 +5524,64 @@
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B42" s="91" t="s">
+      <c r="B42" s="81" t="s">
         <v>220</v>
       </c>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="91"/>
-      <c r="G42" s="91"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
+      <c r="F42" s="81"/>
+      <c r="G42" s="81"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B43" s="92" t="s">
+      <c r="B43" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="C43" s="92" t="s">
+      <c r="C43" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="D43" s="92" t="s">
+      <c r="D43" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="E43" s="92" t="s">
+      <c r="E43" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="F43" s="92" t="s">
+      <c r="F43" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="G43" s="92"/>
+      <c r="G43" s="82"/>
       <c r="H43" s="55" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B44" s="92" t="s">
+      <c r="B44" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="C44" s="92" t="s">
+      <c r="C44" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="92" t="s">
+      <c r="D44" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="E44" s="92" t="s">
+      <c r="E44" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="F44" s="92">
+      <c r="F44" s="82">
         <v>2005</v>
       </c>
-      <c r="G44" s="92"/>
+      <c r="G44" s="82"/>
       <c r="H44" s="6">
         <v>1005</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B45" s="92"/>
-      <c r="C45" s="92"/>
-      <c r="D45" s="92"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
+      <c r="B45" s="82"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="82"/>
+      <c r="G45" s="82"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B46" s="52"/>
@@ -5706,7 +5727,7 @@
         <v>0</v>
       </c>
       <c r="H54" s="40"/>
-      <c r="I54" s="93"/>
+      <c r="I54" s="83"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B55" s="64" t="s">
@@ -5730,7 +5751,7 @@
       <c r="H55" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="I55" s="93"/>
+      <c r="I55" s="83"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B56" s="5" t="s">
@@ -5741,7 +5762,7 @@
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
-      <c r="I56" s="93"/>
+      <c r="I56" s="83"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B57" s="65" t="s">
@@ -5765,7 +5786,7 @@
       <c r="H57" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="I57" s="93"/>
+      <c r="I57" s="83"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B58" s="64" t="s">
@@ -5787,7 +5808,7 @@
         <v>8202</v>
       </c>
       <c r="H58" s="40"/>
-      <c r="I58" s="93"/>
+      <c r="I58" s="83"/>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B59" s="5" t="s">
@@ -5798,7 +5819,7 @@
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
-      <c r="I59" s="93"/>
+      <c r="I59" s="83"/>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B60" s="65" t="s">
@@ -5822,7 +5843,7 @@
       <c r="H60" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I60" s="93" t="s">
+      <c r="I60" s="83" t="s">
         <v>88</v>
       </c>
     </row>
@@ -5845,7 +5866,7 @@
       <c r="G61" s="64">
         <v>8500</v>
       </c>
-      <c r="I61" s="93"/>
+      <c r="I61" s="83"/>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B62" s="5" t="s">
@@ -5856,7 +5877,7 @@
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
-      <c r="I62" s="93"/>
+      <c r="I62" s="83"/>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B63" s="65" t="s">
@@ -5880,7 +5901,7 @@
       <c r="H63" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I63" s="93"/>
+      <c r="I63" s="83"/>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B64" s="42" t="s">
@@ -5901,7 +5922,7 @@
       <c r="G64" s="42">
         <v>8202</v>
       </c>
-      <c r="I64" s="93"/>
+      <c r="I64" s="83"/>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B65" s="41"/>
@@ -5910,7 +5931,7 @@
       <c r="E65" s="41"/>
       <c r="F65" s="41"/>
       <c r="G65" s="41"/>
-      <c r="I65" s="93"/>
+      <c r="I65" s="83"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B66" s="41"/>
@@ -5992,74 +6013,74 @@
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B72" s="71" t="s">
+      <c r="B72" s="111" t="s">
         <v>124</v>
       </c>
-      <c r="C72" s="72"/>
+      <c r="C72" s="112"/>
       <c r="D72" s="51"/>
       <c r="E72" s="51"/>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B73" s="91" t="s">
+      <c r="B73" s="81" t="s">
         <v>221</v>
       </c>
-      <c r="C73" s="91"/>
-      <c r="D73" s="91"/>
-      <c r="E73" s="91"/>
-      <c r="F73" s="91"/>
-      <c r="G73" s="91"/>
+      <c r="C73" s="81"/>
+      <c r="D73" s="81"/>
+      <c r="E73" s="81"/>
+      <c r="F73" s="81"/>
+      <c r="G73" s="81"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B74" s="92" t="s">
+      <c r="B74" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="C74" s="92" t="s">
+      <c r="C74" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="D74" s="92" t="s">
+      <c r="D74" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="E74" s="92" t="s">
+      <c r="E74" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="F74" s="92" t="s">
+      <c r="F74" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="G74" s="92"/>
+      <c r="G74" s="82"/>
       <c r="H74" s="55" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="C75" s="92" t="s">
+      <c r="C75" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="D75" s="92" t="s">
+      <c r="D75" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="E75" s="92" t="s">
+      <c r="E75" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="F75" s="92">
+      <c r="F75" s="82">
         <v>2006</v>
       </c>
-      <c r="G75" s="92"/>
+      <c r="G75" s="82"/>
       <c r="H75" s="6">
         <v>1006</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B76" s="92"/>
-      <c r="C76" s="92"/>
-      <c r="D76" s="92"/>
-      <c r="E76" s="92"/>
-      <c r="F76" s="92"/>
-      <c r="G76" s="92"/>
+      <c r="B76" s="82"/>
+      <c r="C76" s="82"/>
+      <c r="D76" s="82"/>
+      <c r="E76" s="82"/>
+      <c r="F76" s="82"/>
+      <c r="G76" s="82"/>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B77" s="52"/>
@@ -6179,7 +6200,7 @@
       <c r="H85" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="I85" s="93"/>
+      <c r="I85" s="83"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B86" s="64" t="s">
@@ -6196,7 +6217,7 @@
       <c r="G86" s="64">
         <v>8201</v>
       </c>
-      <c r="I86" s="93"/>
+      <c r="I86" s="83"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B87" s="5" t="s">
@@ -6207,7 +6228,7 @@
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
-      <c r="I87" s="93"/>
+      <c r="I87" s="83"/>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B88" s="65" t="s">
@@ -6227,7 +6248,7 @@
       <c r="H88" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="I88" s="93"/>
+      <c r="I88" s="83"/>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B89" s="64" t="s">
@@ -6245,7 +6266,7 @@
         <v>8202</v>
       </c>
       <c r="H89" s="40"/>
-      <c r="I89" s="93"/>
+      <c r="I89" s="83"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B90" s="5" t="s">
@@ -6256,7 +6277,7 @@
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
-      <c r="I90" s="93"/>
+      <c r="I90" s="83"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B91" s="65" t="s">
@@ -6276,7 +6297,7 @@
       <c r="H91" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I91" s="93" t="s">
+      <c r="I91" s="83" t="s">
         <v>88</v>
       </c>
     </row>
@@ -6295,7 +6316,7 @@
       <c r="G92" s="64">
         <v>8500</v>
       </c>
-      <c r="I92" s="93"/>
+      <c r="I92" s="83"/>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B93" s="5" t="s">
@@ -6306,7 +6327,7 @@
       <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
-      <c r="I93" s="93"/>
+      <c r="I93" s="83"/>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B94" s="65" t="s">
@@ -6326,7 +6347,7 @@
       <c r="H94" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I94" s="93"/>
+      <c r="I94" s="83"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B95" s="42" t="s">
@@ -6343,7 +6364,7 @@
       <c r="G95" s="42">
         <v>8202</v>
       </c>
-      <c r="I95" s="93"/>
+      <c r="I95" s="83"/>
     </row>
     <row r="96" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B96" s="9" t="s">
@@ -6354,7 +6375,7 @@
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
-      <c r="I96" s="93"/>
+      <c r="I96" s="83"/>
     </row>
     <row r="98" spans="2:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="99" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
@@ -6398,74 +6419,74 @@
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B101" s="71" t="s">
+      <c r="B101" s="111" t="s">
         <v>123</v>
       </c>
-      <c r="C101" s="72"/>
+      <c r="C101" s="112"/>
       <c r="D101" s="51"/>
       <c r="E101" s="51"/>
       <c r="F101" s="51"/>
       <c r="G101" s="51"/>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B102" s="91" t="s">
+      <c r="B102" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="C102" s="91"/>
-      <c r="D102" s="91"/>
-      <c r="E102" s="91"/>
-      <c r="F102" s="91"/>
-      <c r="G102" s="91"/>
+      <c r="C102" s="81"/>
+      <c r="D102" s="81"/>
+      <c r="E102" s="81"/>
+      <c r="F102" s="81"/>
+      <c r="G102" s="81"/>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B103" s="92" t="s">
+      <c r="B103" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="C103" s="92" t="s">
+      <c r="C103" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="D103" s="92" t="s">
+      <c r="D103" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="E103" s="92" t="s">
+      <c r="E103" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="F103" s="92" t="s">
+      <c r="F103" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="G103" s="92"/>
+      <c r="G103" s="82"/>
       <c r="H103" s="55" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B104" s="92" t="s">
+      <c r="B104" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="C104" s="92" t="s">
+      <c r="C104" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="D104" s="92" t="s">
+      <c r="D104" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="E104" s="92" t="s">
+      <c r="E104" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="F104" s="92">
+      <c r="F104" s="82">
         <v>2001</v>
       </c>
-      <c r="G104" s="92"/>
+      <c r="G104" s="82"/>
       <c r="H104" s="6">
         <v>1001</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B105" s="92"/>
-      <c r="C105" s="92"/>
-      <c r="D105" s="92"/>
-      <c r="E105" s="92"/>
-      <c r="F105" s="92"/>
-      <c r="G105" s="92"/>
+      <c r="B105" s="82"/>
+      <c r="C105" s="82"/>
+      <c r="D105" s="82"/>
+      <c r="E105" s="82"/>
+      <c r="F105" s="82"/>
+      <c r="G105" s="82"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B106" s="52"/>
@@ -6602,7 +6623,7 @@
       <c r="H114" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I114" s="93"/>
+      <c r="I114" s="83"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B115" s="42" t="s">
@@ -6623,7 +6644,7 @@
       <c r="G115" s="42">
         <v>0</v>
       </c>
-      <c r="I115" s="93"/>
+      <c r="I115" s="83"/>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B116" s="5" t="s">
@@ -6634,7 +6655,7 @@
       <c r="E116" s="5"/>
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
-      <c r="I116" s="93"/>
+      <c r="I116" s="83"/>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B117" s="42" t="s">
@@ -6658,7 +6679,7 @@
       <c r="H117" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="I117" s="93"/>
+      <c r="I117" s="83"/>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B118" s="64" t="s">
@@ -6680,7 +6701,7 @@
         <v>1</v>
       </c>
       <c r="H118" s="40"/>
-      <c r="I118" s="93"/>
+      <c r="I118" s="83"/>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B119" s="5" t="s">
@@ -6691,7 +6712,7 @@
       <c r="E119" s="5"/>
       <c r="F119" s="5"/>
       <c r="G119" s="5"/>
-      <c r="I119" s="93"/>
+      <c r="I119" s="83"/>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B120" s="65" t="s">
@@ -6715,7 +6736,7 @@
       <c r="H120" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="I120" s="93" t="s">
+      <c r="I120" s="83" t="s">
         <v>88</v>
       </c>
     </row>
@@ -6738,7 +6759,7 @@
       <c r="G121" s="64">
         <v>0</v>
       </c>
-      <c r="I121" s="93"/>
+      <c r="I121" s="83"/>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B122" s="5" t="s">
@@ -6749,7 +6770,7 @@
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
       <c r="G122" s="5"/>
-      <c r="I122" s="93"/>
+      <c r="I122" s="83"/>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B123" s="65" t="s">
@@ -6773,7 +6794,7 @@
       <c r="H123" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I123" s="93"/>
+      <c r="I123" s="83"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B124" s="42" t="s">
@@ -6794,7 +6815,7 @@
       <c r="G124" s="42">
         <v>0</v>
       </c>
-      <c r="I124" s="93"/>
+      <c r="I124" s="83"/>
     </row>
     <row r="125" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B125" s="9" t="s">
@@ -6805,7 +6826,7 @@
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
       <c r="G125" s="8"/>
-      <c r="I125" s="93"/>
+      <c r="I125" s="83"/>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.45">
       <c r="I126" s="5"/>
@@ -6863,74 +6884,74 @@
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B131" s="71" t="s">
+      <c r="B131" s="111" t="s">
         <v>123</v>
       </c>
-      <c r="C131" s="72"/>
+      <c r="C131" s="112"/>
       <c r="D131" s="51"/>
       <c r="E131" s="51"/>
       <c r="F131" s="51"/>
       <c r="G131" s="51"/>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B132" s="91" t="s">
+      <c r="B132" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="C132" s="91"/>
-      <c r="D132" s="91"/>
-      <c r="E132" s="91"/>
-      <c r="F132" s="91"/>
-      <c r="G132" s="91"/>
+      <c r="C132" s="81"/>
+      <c r="D132" s="81"/>
+      <c r="E132" s="81"/>
+      <c r="F132" s="81"/>
+      <c r="G132" s="81"/>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B133" s="92" t="s">
+      <c r="B133" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="C133" s="92" t="s">
+      <c r="C133" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="D133" s="92" t="s">
+      <c r="D133" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="E133" s="92" t="s">
+      <c r="E133" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="F133" s="92" t="s">
+      <c r="F133" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="G133" s="92"/>
+      <c r="G133" s="82"/>
       <c r="H133" s="55" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B134" s="92" t="s">
+      <c r="B134" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="C134" s="92" t="s">
+      <c r="C134" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="D134" s="92" t="s">
+      <c r="D134" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="E134" s="92" t="s">
+      <c r="E134" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="F134" s="92">
+      <c r="F134" s="82">
         <v>2002</v>
       </c>
-      <c r="G134" s="92"/>
+      <c r="G134" s="82"/>
       <c r="H134" s="6">
         <v>1002</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B135" s="92"/>
-      <c r="C135" s="92"/>
-      <c r="D135" s="92"/>
-      <c r="E135" s="92"/>
-      <c r="F135" s="92"/>
-      <c r="G135" s="92"/>
+      <c r="B135" s="82"/>
+      <c r="C135" s="82"/>
+      <c r="D135" s="82"/>
+      <c r="E135" s="82"/>
+      <c r="F135" s="82"/>
+      <c r="G135" s="82"/>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B136" s="52"/>
@@ -7067,7 +7088,7 @@
       <c r="H144" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I144" s="93"/>
+      <c r="I144" s="83"/>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B145" s="42" t="s">
@@ -7088,7 +7109,7 @@
       <c r="G145" s="42">
         <v>0</v>
       </c>
-      <c r="I145" s="93"/>
+      <c r="I145" s="83"/>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B146" s="5" t="s">
@@ -7099,7 +7120,7 @@
       <c r="E146" s="5"/>
       <c r="F146" s="5"/>
       <c r="G146" s="5"/>
-      <c r="I146" s="93"/>
+      <c r="I146" s="83"/>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B147" s="42" t="s">
@@ -7123,7 +7144,7 @@
       <c r="H147" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="I147" s="93"/>
+      <c r="I147" s="83"/>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B148" s="64" t="s">
@@ -7145,7 +7166,7 @@
         <v>1</v>
       </c>
       <c r="H148" s="40"/>
-      <c r="I148" s="93"/>
+      <c r="I148" s="83"/>
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B149" s="5" t="s">
@@ -7156,7 +7177,7 @@
       <c r="E149" s="5"/>
       <c r="F149" s="5"/>
       <c r="G149" s="5"/>
-      <c r="I149" s="93"/>
+      <c r="I149" s="83"/>
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B150" s="65" t="s">
@@ -7180,7 +7201,7 @@
       <c r="H150" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="I150" s="93" t="s">
+      <c r="I150" s="83" t="s">
         <v>88</v>
       </c>
     </row>
@@ -7203,7 +7224,7 @@
       <c r="G151" s="64">
         <v>0</v>
       </c>
-      <c r="I151" s="93"/>
+      <c r="I151" s="83"/>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B152" s="5" t="s">
@@ -7214,7 +7235,7 @@
       <c r="E152" s="5"/>
       <c r="F152" s="5"/>
       <c r="G152" s="5"/>
-      <c r="I152" s="93"/>
+      <c r="I152" s="83"/>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B153" s="65" t="s">
@@ -7238,7 +7259,7 @@
       <c r="H153" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I153" s="93"/>
+      <c r="I153" s="83"/>
     </row>
     <row r="154" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B154" s="42" t="s">
@@ -7259,7 +7280,7 @@
       <c r="G154" s="42">
         <v>0</v>
       </c>
-      <c r="I154" s="93"/>
+      <c r="I154" s="83"/>
     </row>
     <row r="155" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B155" s="9" t="s">
@@ -7270,7 +7291,7 @@
       <c r="E155" s="7"/>
       <c r="F155" s="7"/>
       <c r="G155" s="8"/>
-      <c r="I155" s="93"/>
+      <c r="I155" s="83"/>
     </row>
     <row r="156" spans="2:9" x14ac:dyDescent="0.45">
       <c r="I156" s="5"/>
@@ -7320,74 +7341,74 @@
       </c>
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B161" s="71" t="s">
+      <c r="B161" s="111" t="s">
         <v>123</v>
       </c>
-      <c r="C161" s="72"/>
+      <c r="C161" s="112"/>
       <c r="D161" s="51"/>
       <c r="E161" s="51"/>
       <c r="F161" s="51"/>
       <c r="G161" s="51"/>
     </row>
     <row r="162" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B162" s="91" t="s">
+      <c r="B162" s="81" t="s">
         <v>223</v>
       </c>
-      <c r="C162" s="91"/>
-      <c r="D162" s="91"/>
-      <c r="E162" s="91"/>
-      <c r="F162" s="91"/>
-      <c r="G162" s="91"/>
+      <c r="C162" s="81"/>
+      <c r="D162" s="81"/>
+      <c r="E162" s="81"/>
+      <c r="F162" s="81"/>
+      <c r="G162" s="81"/>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B163" s="92" t="s">
+      <c r="B163" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="C163" s="92" t="s">
+      <c r="C163" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="D163" s="92" t="s">
+      <c r="D163" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="E163" s="92" t="s">
+      <c r="E163" s="82" t="s">
         <v>120</v>
       </c>
-      <c r="F163" s="92" t="s">
+      <c r="F163" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="G163" s="92"/>
+      <c r="G163" s="82"/>
       <c r="H163" s="55" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="164" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B164" s="92" t="s">
+      <c r="B164" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="C164" s="92" t="s">
+      <c r="C164" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="D164" s="92" t="s">
+      <c r="D164" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="E164" s="92" t="s">
+      <c r="E164" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="F164" s="92">
+      <c r="F164" s="82">
         <v>2003</v>
       </c>
-      <c r="G164" s="92"/>
+      <c r="G164" s="82"/>
       <c r="H164" s="6">
         <v>1003</v>
       </c>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B165" s="92"/>
-      <c r="C165" s="92"/>
-      <c r="D165" s="92"/>
-      <c r="E165" s="92"/>
-      <c r="F165" s="92"/>
-      <c r="G165" s="92"/>
+      <c r="B165" s="82"/>
+      <c r="C165" s="82"/>
+      <c r="D165" s="82"/>
+      <c r="E165" s="82"/>
+      <c r="F165" s="82"/>
+      <c r="G165" s="82"/>
     </row>
     <row r="166" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B166" s="52"/>
@@ -7504,7 +7525,7 @@
       <c r="H174" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I174" s="93"/>
+      <c r="I174" s="83"/>
     </row>
     <row r="175" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B175" s="42" t="s">
@@ -7521,7 +7542,7 @@
       </c>
       <c r="F175" s="42"/>
       <c r="G175" s="42"/>
-      <c r="I175" s="93"/>
+      <c r="I175" s="83"/>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B176" s="5" t="s">
@@ -7532,7 +7553,7 @@
       <c r="E176" s="5"/>
       <c r="F176" s="5"/>
       <c r="G176" s="5"/>
-      <c r="I176" s="93"/>
+      <c r="I176" s="83"/>
     </row>
     <row r="177" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B177" s="42" t="s">
@@ -7552,7 +7573,7 @@
       <c r="H177" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="I177" s="93"/>
+      <c r="I177" s="83"/>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B178" s="64" t="s">
@@ -7570,7 +7591,7 @@
       <c r="F178" s="64"/>
       <c r="G178" s="64"/>
       <c r="H178" s="40"/>
-      <c r="I178" s="93"/>
+      <c r="I178" s="83"/>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B179" s="5" t="s">
@@ -7581,7 +7602,7 @@
       <c r="E179" s="5"/>
       <c r="F179" s="5"/>
       <c r="G179" s="5"/>
-      <c r="I179" s="93"/>
+      <c r="I179" s="83"/>
     </row>
     <row r="180" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B180" s="65" t="s">
@@ -7601,7 +7622,7 @@
       <c r="H180" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="I180" s="93" t="s">
+      <c r="I180" s="83" t="s">
         <v>88</v>
       </c>
     </row>
@@ -7620,7 +7641,7 @@
       </c>
       <c r="F181" s="69"/>
       <c r="G181" s="69"/>
-      <c r="I181" s="93"/>
+      <c r="I181" s="83"/>
     </row>
     <row r="182" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B182" s="5" t="s">
@@ -7631,7 +7652,7 @@
       <c r="E182" s="5"/>
       <c r="F182" s="5" ph="1"/>
       <c r="G182" s="5"/>
-      <c r="I182" s="93"/>
+      <c r="I182" s="83"/>
     </row>
     <row r="183" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B183" s="65" t="s">
@@ -7651,7 +7672,7 @@
       <c r="H183" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I183" s="93"/>
+      <c r="I183" s="83"/>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B184" s="42" t="s">
@@ -7668,7 +7689,7 @@
       </c>
       <c r="F184" s="43"/>
       <c r="G184" s="43"/>
-      <c r="I184" s="93"/>
+      <c r="I184" s="83"/>
     </row>
     <row r="185" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B185" s="9" t="s">
@@ -7680,7 +7701,7 @@
       <c r="F185" s="7"/>
       <c r="G185" s="8"/>
       <c r="H185" s="40"/>
-      <c r="I185" s="93"/>
+      <c r="I185" s="83"/>
     </row>
     <row r="212" ht="249" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
@@ -7721,7 +7742,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="76" t="s">
         <v>184</v>
       </c>
     </row>
@@ -7773,10 +7794,10 @@
       <c r="C4" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="78"/>
+      <c r="E4" s="72"/>
       <c r="F4" s="56" t="s">
         <v>108</v>
       </c>
@@ -7803,10 +7824,10 @@
       <c r="C5" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="75" t="s">
         <v>147</v>
       </c>
       <c r="F5" s="56" t="s">
@@ -7829,10 +7850,10 @@
       <c r="C6" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="E6" s="82" t="s">
+      <c r="E6" s="75" t="s">
         <v>146</v>
       </c>
       <c r="F6" s="56" t="s">
@@ -7855,10 +7876,10 @@
       <c r="C7" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="82" t="s">
+      <c r="E7" s="75" t="s">
         <v>191</v>
       </c>
       <c r="F7" s="56"/>
@@ -7879,13 +7900,13 @@
       <c r="C8" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="2" t="s">
         <v>192</v>
       </c>
       <c r="E8" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="73" t="s">
         <v>196</v>
       </c>
       <c r="G8" s="56"/>
@@ -7905,11 +7926,11 @@
       <c r="C9" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="79" t="s">
+      <c r="E9" s="77"/>
+      <c r="F9" s="73" t="s">
         <v>151</v>
       </c>
       <c r="G9" s="56"/>
@@ -7929,10 +7950,10 @@
       <c r="C10" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="E10" s="85"/>
+      <c r="E10" s="78"/>
       <c r="F10" s="56" t="s">
         <v>196</v>
       </c>
@@ -7950,14 +7971,14 @@
       <c r="B11" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="56" t="s">
         <v>198</v>
       </c>
       <c r="E11" s="56"/>
-      <c r="F11" s="86" t="s">
+      <c r="F11" s="56" t="s">
         <v>196</v>
       </c>
       <c r="G11" s="56"/>
@@ -7974,14 +7995,14 @@
       <c r="B12" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="56" t="s">
         <v>197</v>
       </c>
       <c r="E12" s="56"/>
-      <c r="F12" s="86" t="s">
+      <c r="F12" s="56" t="s">
         <v>196</v>
       </c>
       <c r="G12" s="56"/>
@@ -7995,19 +8016,19 @@
       <c r="A13" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="56" t="s">
         <v>202</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="86" t="s">
+      <c r="D13" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="E13" s="86" t="s">
+      <c r="E13" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="F13" s="86" t="s">
+      <c r="F13" s="56" t="s">
         <v>147</v>
       </c>
       <c r="G13" s="56"/>
@@ -8018,22 +8039,22 @@
       <c r="L13" s="56"/>
     </row>
     <row r="14" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="84" t="s">
         <v>225</v>
       </c>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="E14" s="86" t="s">
+      <c r="E14" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="86" t="s">
+      <c r="F14" s="56" t="s">
         <v>147</v>
       </c>
       <c r="G14" s="56"/>

</xml_diff>